<commit_message>
add : cas d'usage (incomplet)
</commit_message>
<xml_diff>
--- a/doc/chiffrier_sim_vie.xlsx
+++ b/doc/chiffrier_sim_vie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\travail\sim_vie-420-C41-IN-\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC820651-6ADF-4CF2-98E5-A323E1288331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203274B2-E6AE-4AFE-A266-DD096DD4D582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Méthodes SCRUM" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="282">
   <si>
     <t>Chiffrier de documentation de projets</t>
   </si>
@@ -1107,6 +1107,121 @@
   <si>
     <t>s'éveiller</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">Notes </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Pour information supplémentaire</t>
+    </r>
+  </si>
+  <si>
+    <t>Utiliser le IF pour des sections conditionnelles</t>
+  </si>
+  <si>
+    <t>Tâche complète</t>
+  </si>
+  <si>
+    <t>Rôle</t>
+  </si>
+  <si>
+    <t>Changement de température</t>
+  </si>
+  <si>
+    <t>Changement du taux d'humidité</t>
+  </si>
+  <si>
+    <t>usager</t>
+  </si>
+  <si>
+    <t>Ajout de nuages de pression</t>
+  </si>
+  <si>
+    <t>Modification de nuages de pression</t>
+  </si>
+  <si>
+    <t>Changement de rapport nourriture / organisme</t>
+  </si>
+  <si>
+    <t>Changement de rapport terre / eau</t>
+  </si>
+  <si>
+    <t>Changement de la durée des cycles</t>
+  </si>
+  <si>
+    <t>(usager, environnement, organisme)</t>
+  </si>
+  <si>
+    <t>Changement de la taille du monde</t>
+  </si>
+  <si>
+    <t>Faire défiler l'écran (Scroll)</t>
+  </si>
+  <si>
+    <t>Agrandir ou réduire la fenêtre (Zoom in - Zoom out)</t>
+  </si>
+  <si>
+    <t>environnement</t>
+  </si>
+  <si>
+    <t>Déplacement des nuages de pression</t>
+  </si>
+  <si>
+    <t>Génération de nourriture</t>
+  </si>
+  <si>
+    <t>Changement de cycle</t>
+  </si>
+  <si>
+    <t>organisme</t>
+  </si>
+  <si>
+    <t>Manger</t>
+  </si>
+  <si>
+    <t>Boire</t>
+  </si>
+  <si>
+    <t>Déféquer</t>
+  </si>
+  <si>
+    <t>Mourir</t>
+  </si>
+  <si>
+    <t>Donner naissance</t>
+  </si>
+  <si>
+    <t>Se reproduire</t>
+  </si>
+  <si>
+    <t>Se déplacer</t>
+  </si>
+  <si>
+    <t>Se mettre en état de cryptobiose</t>
+  </si>
+  <si>
+    <t>Dormir / Se réveiller</t>
+  </si>
+  <si>
+    <t>Choisir une direction</t>
+  </si>
+  <si>
+    <t>Machine (Organisme)</t>
+  </si>
+  <si>
+    <t>Machine (Environnement)</t>
+  </si>
 </sst>
 </file>
 
@@ -1117,7 +1232,7 @@
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="166" formatCode="m/d/yy"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1266,6 +1381,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1281,7 +1403,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="60">
+  <borders count="72">
     <border>
       <left/>
       <right/>
@@ -1940,11 +2062,167 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="182">
+  <cellXfs count="234">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2247,11 +2525,84 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2290,78 +2641,143 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="71" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3059,22 +3475,22 @@
       </c>
     </row>
     <row r="36" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F36" s="142"/>
-      <c r="G36" s="143"/>
-      <c r="H36" s="143"/>
-      <c r="I36" s="143"/>
+      <c r="F36" s="165"/>
+      <c r="G36" s="166"/>
+      <c r="H36" s="166"/>
+      <c r="I36" s="166"/>
     </row>
     <row r="37" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F37" s="143"/>
-      <c r="G37" s="143"/>
-      <c r="H37" s="143"/>
-      <c r="I37" s="143"/>
+      <c r="F37" s="166"/>
+      <c r="G37" s="166"/>
+      <c r="H37" s="166"/>
+      <c r="I37" s="166"/>
     </row>
     <row r="38" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F38" s="143"/>
-      <c r="G38" s="143"/>
-      <c r="H38" s="143"/>
-      <c r="I38" s="143"/>
+      <c r="F38" s="166"/>
+      <c r="G38" s="166"/>
+      <c r="H38" s="166"/>
+      <c r="I38" s="166"/>
     </row>
     <row r="39" spans="6:9" ht="17.25" customHeight="1">
       <c r="F39" s="82"/>
@@ -3083,22 +3499,22 @@
       <c r="I39" s="82"/>
     </row>
     <row r="40" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F40" s="142"/>
-      <c r="G40" s="143"/>
-      <c r="H40" s="143"/>
-      <c r="I40" s="143"/>
+      <c r="F40" s="165"/>
+      <c r="G40" s="166"/>
+      <c r="H40" s="166"/>
+      <c r="I40" s="166"/>
     </row>
     <row r="41" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F41" s="143"/>
-      <c r="G41" s="143"/>
-      <c r="H41" s="143"/>
-      <c r="I41" s="143"/>
+      <c r="F41" s="166"/>
+      <c r="G41" s="166"/>
+      <c r="H41" s="166"/>
+      <c r="I41" s="166"/>
     </row>
     <row r="42" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F42" s="143"/>
-      <c r="G42" s="143"/>
-      <c r="H42" s="143"/>
-      <c r="I42" s="143"/>
+      <c r="F42" s="166"/>
+      <c r="G42" s="166"/>
+      <c r="H42" s="166"/>
+      <c r="I42" s="166"/>
     </row>
     <row r="43" spans="6:9" ht="17.25" customHeight="1">
       <c r="F43" s="82"/>
@@ -3113,34 +3529,34 @@
       <c r="I44" s="82"/>
     </row>
     <row r="45" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F45" s="142"/>
-      <c r="G45" s="143"/>
-      <c r="H45" s="143"/>
-      <c r="I45" s="143"/>
+      <c r="F45" s="165"/>
+      <c r="G45" s="166"/>
+      <c r="H45" s="166"/>
+      <c r="I45" s="166"/>
     </row>
     <row r="46" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F46" s="143"/>
-      <c r="G46" s="143"/>
-      <c r="H46" s="143"/>
-      <c r="I46" s="143"/>
+      <c r="F46" s="166"/>
+      <c r="G46" s="166"/>
+      <c r="H46" s="166"/>
+      <c r="I46" s="166"/>
     </row>
     <row r="47" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F47" s="143"/>
-      <c r="G47" s="143"/>
-      <c r="H47" s="143"/>
-      <c r="I47" s="143"/>
+      <c r="F47" s="166"/>
+      <c r="G47" s="166"/>
+      <c r="H47" s="166"/>
+      <c r="I47" s="166"/>
     </row>
     <row r="48" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F48" s="143"/>
-      <c r="G48" s="143"/>
-      <c r="H48" s="143"/>
-      <c r="I48" s="143"/>
+      <c r="F48" s="166"/>
+      <c r="G48" s="166"/>
+      <c r="H48" s="166"/>
+      <c r="I48" s="166"/>
     </row>
     <row r="49" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F49" s="143"/>
-      <c r="G49" s="143"/>
-      <c r="H49" s="143"/>
-      <c r="I49" s="143"/>
+      <c r="F49" s="166"/>
+      <c r="G49" s="166"/>
+      <c r="H49" s="166"/>
+      <c r="I49" s="166"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3159,7 +3575,7 @@
   </sheetPr>
   <dimension ref="B2:H99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
@@ -3263,740 +3679,740 @@
       </c>
     </row>
     <row r="13" spans="2:8" ht="12.75" customHeight="1">
-      <c r="B13" s="157" t="s">
+      <c r="B13" s="167" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="159"/>
+      <c r="C13" s="142"/>
       <c r="D13" s="15"/>
       <c r="E13" s="25"/>
-      <c r="H13" s="180"/>
+      <c r="H13" s="163"/>
     </row>
     <row r="14" spans="2:8" ht="12.75" customHeight="1">
-      <c r="B14" s="158"/>
-      <c r="C14" s="160" t="s">
+      <c r="B14" s="168"/>
+      <c r="C14" s="143" t="s">
         <v>158</v>
       </c>
-      <c r="D14" s="160" t="s">
+      <c r="D14" s="143" t="s">
         <v>158</v>
       </c>
-      <c r="E14" s="160" t="s">
+      <c r="E14" s="143" t="s">
         <v>158</v>
       </c>
-      <c r="H14" s="180"/>
+      <c r="H14" s="163"/>
     </row>
     <row r="15" spans="2:8" ht="12.75" customHeight="1">
-      <c r="B15" s="158"/>
-      <c r="C15" s="163"/>
-      <c r="D15" s="161"/>
-      <c r="E15" s="162"/>
+      <c r="B15" s="168"/>
+      <c r="C15" s="146"/>
+      <c r="D15" s="144"/>
+      <c r="E15" s="145"/>
     </row>
     <row r="16" spans="2:8" ht="12.75" customHeight="1">
-      <c r="B16" s="158"/>
-      <c r="C16" s="173" t="s">
+      <c r="B16" s="168"/>
+      <c r="C16" s="156" t="s">
         <v>225</v>
       </c>
-      <c r="D16" s="174" t="s">
+      <c r="D16" s="157" t="s">
         <v>163</v>
       </c>
-      <c r="E16" s="162" t="s">
+      <c r="E16" s="145" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B17" s="144"/>
-      <c r="C17" s="163" t="s">
+      <c r="B17" s="169"/>
+      <c r="C17" s="146" t="s">
         <v>155</v>
       </c>
-      <c r="D17" s="161"/>
-      <c r="E17" s="162"/>
+      <c r="D17" s="144"/>
+      <c r="E17" s="145"/>
     </row>
     <row r="18" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B18" s="144"/>
-      <c r="C18" s="173" t="s">
+      <c r="B18" s="169"/>
+      <c r="C18" s="156" t="s">
         <v>226</v>
       </c>
-      <c r="D18" s="161"/>
-      <c r="E18" s="175" t="s">
+      <c r="D18" s="144"/>
+      <c r="E18" s="158" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B19" s="144"/>
-      <c r="C19" s="163"/>
-      <c r="D19" s="161"/>
-      <c r="E19" s="162"/>
+      <c r="B19" s="169"/>
+      <c r="C19" s="146"/>
+      <c r="D19" s="144"/>
+      <c r="E19" s="145"/>
     </row>
     <row r="20" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B20" s="144"/>
-      <c r="C20" s="160" t="s">
+      <c r="B20" s="169"/>
+      <c r="C20" s="143" t="s">
         <v>159</v>
       </c>
-      <c r="D20" s="160" t="s">
+      <c r="D20" s="143" t="s">
         <v>159</v>
       </c>
-      <c r="E20" s="160" t="s">
+      <c r="E20" s="143" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B21" s="144"/>
-      <c r="C21" s="163"/>
-      <c r="D21" s="161"/>
-      <c r="E21" s="162"/>
+      <c r="B21" s="169"/>
+      <c r="C21" s="146"/>
+      <c r="D21" s="144"/>
+      <c r="E21" s="145"/>
     </row>
     <row r="22" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B22" s="144"/>
-      <c r="C22" s="173" t="s">
+      <c r="B22" s="169"/>
+      <c r="C22" s="156" t="s">
         <v>228</v>
       </c>
-      <c r="D22" s="161" t="s">
+      <c r="D22" s="144" t="s">
         <v>161</v>
       </c>
-      <c r="E22" s="175" t="s">
+      <c r="E22" s="158" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B23" s="144"/>
-      <c r="C23" s="178" t="s">
+      <c r="B23" s="169"/>
+      <c r="C23" s="161" t="s">
         <v>164</v>
       </c>
-      <c r="D23" s="179" t="s">
+      <c r="D23" s="162" t="s">
         <v>165</v>
       </c>
-      <c r="E23" s="177" t="s">
+      <c r="E23" s="160" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B24" s="144"/>
-      <c r="C24" s="163"/>
-      <c r="D24" s="174" t="s">
+      <c r="B24" s="169"/>
+      <c r="C24" s="146"/>
+      <c r="D24" s="157" t="s">
         <v>230</v>
       </c>
-      <c r="E24" s="175"/>
+      <c r="E24" s="158"/>
     </row>
     <row r="25" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B25" s="144"/>
-      <c r="C25" s="173"/>
-      <c r="D25" s="174" t="s">
+      <c r="B25" s="169"/>
+      <c r="C25" s="156"/>
+      <c r="D25" s="157" t="s">
         <v>167</v>
       </c>
-      <c r="E25" s="175"/>
+      <c r="E25" s="158"/>
     </row>
     <row r="26" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B26" s="144"/>
-      <c r="C26" s="173" t="s">
+      <c r="B26" s="169"/>
+      <c r="C26" s="156" t="s">
         <v>168</v>
       </c>
-      <c r="D26" s="161"/>
-      <c r="E26" s="175" t="s">
+      <c r="D26" s="144"/>
+      <c r="E26" s="158" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B27" s="144"/>
-      <c r="C27" s="173" t="s">
+      <c r="B27" s="169"/>
+      <c r="C27" s="156" t="s">
         <v>170</v>
       </c>
-      <c r="D27" s="161"/>
-      <c r="E27" s="175" t="s">
+      <c r="D27" s="144"/>
+      <c r="E27" s="158" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B28" s="144"/>
-      <c r="C28" s="163"/>
-      <c r="D28" s="161"/>
-      <c r="E28" s="162"/>
+      <c r="B28" s="169"/>
+      <c r="C28" s="146"/>
+      <c r="D28" s="144"/>
+      <c r="E28" s="145"/>
     </row>
     <row r="29" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B29" s="144"/>
-      <c r="C29" s="160" t="s">
+      <c r="B29" s="169"/>
+      <c r="C29" s="143" t="s">
         <v>172</v>
       </c>
-      <c r="D29" s="161"/>
-      <c r="E29" s="162"/>
+      <c r="D29" s="144"/>
+      <c r="E29" s="145"/>
     </row>
     <row r="30" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B30" s="144"/>
-      <c r="C30" s="163"/>
-      <c r="D30" s="161"/>
-      <c r="E30" s="162"/>
+      <c r="B30" s="169"/>
+      <c r="C30" s="146"/>
+      <c r="D30" s="144"/>
+      <c r="E30" s="145"/>
     </row>
     <row r="31" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B31" s="144"/>
-      <c r="C31" s="173" t="s">
+      <c r="B31" s="169"/>
+      <c r="C31" s="156" t="s">
         <v>173</v>
       </c>
-      <c r="D31" s="174" t="s">
+      <c r="D31" s="157" t="s">
         <v>178</v>
       </c>
-      <c r="E31" s="162"/>
+      <c r="E31" s="145"/>
     </row>
     <row r="32" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B32" s="144"/>
-      <c r="C32" s="173" t="s">
+      <c r="B32" s="169"/>
+      <c r="C32" s="156" t="s">
         <v>174</v>
       </c>
-      <c r="D32" s="161"/>
-      <c r="E32" s="162"/>
+      <c r="D32" s="144"/>
+      <c r="E32" s="145"/>
     </row>
     <row r="33" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B33" s="144"/>
-      <c r="C33" s="173" t="s">
+      <c r="B33" s="169"/>
+      <c r="C33" s="156" t="s">
         <v>175</v>
       </c>
-      <c r="D33" s="161"/>
-      <c r="E33" s="162"/>
+      <c r="D33" s="144"/>
+      <c r="E33" s="145"/>
     </row>
     <row r="34" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B34" s="144"/>
-      <c r="C34" s="173" t="s">
+      <c r="B34" s="169"/>
+      <c r="C34" s="156" t="s">
         <v>176</v>
       </c>
-      <c r="D34" s="161"/>
-      <c r="E34" s="162"/>
+      <c r="D34" s="144"/>
+      <c r="E34" s="145"/>
     </row>
     <row r="35" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B35" s="144"/>
-      <c r="C35" s="173" t="s">
+      <c r="B35" s="169"/>
+      <c r="C35" s="156" t="s">
         <v>177</v>
       </c>
-      <c r="D35" s="161"/>
-      <c r="E35" s="162"/>
+      <c r="D35" s="144"/>
+      <c r="E35" s="145"/>
     </row>
     <row r="36" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B36" s="144"/>
-      <c r="C36" s="173"/>
-      <c r="D36" s="174"/>
-      <c r="E36" s="162"/>
+      <c r="B36" s="169"/>
+      <c r="C36" s="156"/>
+      <c r="D36" s="157"/>
+      <c r="E36" s="145"/>
     </row>
     <row r="37" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B37" s="144"/>
-      <c r="C37" s="173" t="s">
+      <c r="B37" s="169"/>
+      <c r="C37" s="156" t="s">
         <v>231</v>
       </c>
-      <c r="D37" s="161"/>
-      <c r="E37" s="162"/>
+      <c r="D37" s="144"/>
+      <c r="E37" s="145"/>
     </row>
     <row r="38" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B38" s="144"/>
-      <c r="C38" s="173" t="s">
+      <c r="B38" s="169"/>
+      <c r="C38" s="156" t="s">
         <v>181</v>
       </c>
-      <c r="D38" s="161"/>
-      <c r="E38" s="162"/>
+      <c r="D38" s="144"/>
+      <c r="E38" s="145"/>
     </row>
     <row r="39" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B39" s="144"/>
-      <c r="C39" s="173" t="s">
+      <c r="B39" s="169"/>
+      <c r="C39" s="156" t="s">
         <v>179</v>
       </c>
-      <c r="D39" s="161"/>
-      <c r="E39" s="175" t="s">
+      <c r="D39" s="144"/>
+      <c r="E39" s="158" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="40" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B40" s="144"/>
-      <c r="C40" s="173"/>
-      <c r="D40" s="161"/>
-      <c r="E40" s="162"/>
+      <c r="B40" s="169"/>
+      <c r="C40" s="156"/>
+      <c r="D40" s="144"/>
+      <c r="E40" s="145"/>
     </row>
     <row r="41" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B41" s="144"/>
-      <c r="C41" s="160" t="s">
+      <c r="B41" s="169"/>
+      <c r="C41" s="143" t="s">
         <v>182</v>
       </c>
-      <c r="D41" s="161"/>
-      <c r="E41" s="162"/>
+      <c r="D41" s="144"/>
+      <c r="E41" s="145"/>
     </row>
     <row r="42" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B42" s="144"/>
-      <c r="C42" s="173"/>
-      <c r="D42" s="161"/>
-      <c r="E42" s="162"/>
+      <c r="B42" s="169"/>
+      <c r="C42" s="156"/>
+      <c r="D42" s="144"/>
+      <c r="E42" s="145"/>
     </row>
     <row r="43" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B43" s="144"/>
-      <c r="C43" s="173" t="s">
+      <c r="B43" s="169"/>
+      <c r="C43" s="156" t="s">
         <v>183</v>
       </c>
-      <c r="D43" s="161"/>
-      <c r="E43" s="162"/>
+      <c r="D43" s="144"/>
+      <c r="E43" s="145"/>
     </row>
     <row r="44" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B44" s="144"/>
-      <c r="C44" s="173" t="s">
+      <c r="B44" s="169"/>
+      <c r="C44" s="156" t="s">
         <v>155</v>
       </c>
-      <c r="D44" s="176" t="s">
+      <c r="D44" s="159" t="s">
         <v>184</v>
       </c>
-      <c r="E44" s="162"/>
+      <c r="E44" s="145"/>
     </row>
     <row r="45" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B45" s="144"/>
-      <c r="C45" s="173" t="s">
+      <c r="B45" s="169"/>
+      <c r="C45" s="156" t="s">
         <v>185</v>
       </c>
-      <c r="D45" s="176" t="s">
+      <c r="D45" s="159" t="s">
         <v>186</v>
       </c>
-      <c r="E45" s="162"/>
+      <c r="E45" s="145"/>
     </row>
     <row r="46" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B46" s="144"/>
-      <c r="C46" s="173" t="s">
+      <c r="B46" s="169"/>
+      <c r="C46" s="156" t="s">
         <v>187</v>
       </c>
-      <c r="D46" s="176" t="s">
+      <c r="D46" s="159" t="s">
         <v>188</v>
       </c>
-      <c r="E46" s="162"/>
+      <c r="E46" s="145"/>
     </row>
     <row r="47" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B47" s="144"/>
-      <c r="C47" s="173" t="s">
+      <c r="B47" s="169"/>
+      <c r="C47" s="156" t="s">
         <v>189</v>
       </c>
-      <c r="D47" s="161"/>
-      <c r="E47" s="177" t="s">
+      <c r="D47" s="144"/>
+      <c r="E47" s="160" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="48" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B48" s="144"/>
-      <c r="C48" s="178" t="s">
+      <c r="B48" s="169"/>
+      <c r="C48" s="161" t="s">
         <v>191</v>
       </c>
-      <c r="D48" s="161"/>
-      <c r="E48" s="162"/>
+      <c r="D48" s="144"/>
+      <c r="E48" s="145"/>
     </row>
     <row r="49" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B49" s="144"/>
-      <c r="C49" s="178" t="s">
+      <c r="B49" s="169"/>
+      <c r="C49" s="161" t="s">
         <v>192</v>
       </c>
-      <c r="D49" s="161"/>
-      <c r="E49" s="162"/>
+      <c r="D49" s="144"/>
+      <c r="E49" s="145"/>
     </row>
     <row r="50" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B50" s="144"/>
-      <c r="C50" s="173"/>
-      <c r="D50" s="161"/>
-      <c r="E50" s="162"/>
+      <c r="B50" s="169"/>
+      <c r="C50" s="156"/>
+      <c r="D50" s="144"/>
+      <c r="E50" s="145"/>
     </row>
     <row r="51" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B51" s="144"/>
-      <c r="C51" s="160" t="s">
+      <c r="B51" s="169"/>
+      <c r="C51" s="143" t="s">
         <v>193</v>
       </c>
-      <c r="D51" s="161"/>
-      <c r="E51" s="162"/>
+      <c r="D51" s="144"/>
+      <c r="E51" s="145"/>
     </row>
     <row r="52" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B52" s="144"/>
-      <c r="C52" s="173"/>
-      <c r="D52" s="161"/>
-      <c r="E52" s="162"/>
+      <c r="B52" s="169"/>
+      <c r="C52" s="156"/>
+      <c r="D52" s="144"/>
+      <c r="E52" s="145"/>
     </row>
     <row r="53" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B53" s="144"/>
-      <c r="C53" s="173" t="s">
+      <c r="B53" s="169"/>
+      <c r="C53" s="156" t="s">
         <v>194</v>
       </c>
-      <c r="D53" s="161"/>
-      <c r="E53" s="177" t="s">
+      <c r="D53" s="144"/>
+      <c r="E53" s="160" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="54" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B54" s="144"/>
-      <c r="C54" s="173" t="s">
+      <c r="B54" s="169"/>
+      <c r="C54" s="156" t="s">
         <v>196</v>
       </c>
-      <c r="D54" s="161"/>
-      <c r="E54" s="162"/>
+      <c r="D54" s="144"/>
+      <c r="E54" s="145"/>
     </row>
     <row r="55" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B55" s="144"/>
-      <c r="C55" s="173" t="s">
+      <c r="B55" s="169"/>
+      <c r="C55" s="156" t="s">
         <v>197</v>
       </c>
-      <c r="D55" s="161"/>
-      <c r="E55" s="162"/>
+      <c r="D55" s="144"/>
+      <c r="E55" s="145"/>
     </row>
     <row r="56" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B56" s="144"/>
-      <c r="C56" s="173" t="s">
+      <c r="B56" s="169"/>
+      <c r="C56" s="156" t="s">
         <v>198</v>
       </c>
-      <c r="D56" s="161"/>
-      <c r="E56" s="162"/>
+      <c r="D56" s="144"/>
+      <c r="E56" s="145"/>
     </row>
     <row r="57" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B57" s="144"/>
-      <c r="C57" s="173" t="s">
+      <c r="B57" s="169"/>
+      <c r="C57" s="156" t="s">
         <v>199</v>
       </c>
-      <c r="D57" s="161"/>
-      <c r="E57" s="162"/>
+      <c r="D57" s="144"/>
+      <c r="E57" s="145"/>
     </row>
     <row r="58" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B58" s="144"/>
-      <c r="C58" s="173" t="s">
+      <c r="B58" s="169"/>
+      <c r="C58" s="156" t="s">
         <v>200</v>
       </c>
-      <c r="D58" s="174" t="s">
+      <c r="D58" s="157" t="s">
         <v>201</v>
       </c>
-      <c r="E58" s="162"/>
+      <c r="E58" s="145"/>
     </row>
     <row r="59" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B59" s="144"/>
-      <c r="C59" s="173" t="s">
+      <c r="B59" s="169"/>
+      <c r="C59" s="156" t="s">
         <v>192</v>
       </c>
-      <c r="D59" s="176" t="s">
+      <c r="D59" s="159" t="s">
         <v>202</v>
       </c>
-      <c r="E59" s="162"/>
+      <c r="E59" s="145"/>
     </row>
     <row r="60" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B60" s="144"/>
-      <c r="C60" s="173" t="s">
+      <c r="B60" s="169"/>
+      <c r="C60" s="156" t="s">
         <v>203</v>
       </c>
-      <c r="D60" s="161"/>
-      <c r="E60" s="162"/>
+      <c r="D60" s="144"/>
+      <c r="E60" s="145"/>
     </row>
     <row r="61" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B61" s="144"/>
-      <c r="C61" s="173" t="s">
+      <c r="B61" s="169"/>
+      <c r="C61" s="156" t="s">
         <v>204</v>
       </c>
-      <c r="D61" s="161"/>
-      <c r="E61" s="177" t="s">
+      <c r="D61" s="144"/>
+      <c r="E61" s="160" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="62" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B62" s="144"/>
-      <c r="C62" s="173" t="s">
+      <c r="B62" s="169"/>
+      <c r="C62" s="156" t="s">
         <v>206</v>
       </c>
-      <c r="D62" s="161"/>
-      <c r="E62" s="162"/>
+      <c r="D62" s="144"/>
+      <c r="E62" s="145"/>
     </row>
     <row r="63" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B63" s="144"/>
-      <c r="C63" s="173"/>
-      <c r="D63" s="161"/>
-      <c r="E63" s="162"/>
+      <c r="B63" s="169"/>
+      <c r="C63" s="156"/>
+      <c r="D63" s="144"/>
+      <c r="E63" s="145"/>
     </row>
     <row r="64" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B64" s="144"/>
-      <c r="C64" s="160" t="s">
+      <c r="B64" s="169"/>
+      <c r="C64" s="143" t="s">
         <v>207</v>
       </c>
-      <c r="D64" s="161"/>
-      <c r="E64" s="162"/>
+      <c r="D64" s="144"/>
+      <c r="E64" s="145"/>
     </row>
     <row r="65" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B65" s="144"/>
-      <c r="C65" s="173"/>
-      <c r="D65" s="161"/>
-      <c r="E65" s="162"/>
+      <c r="B65" s="169"/>
+      <c r="C65" s="156"/>
+      <c r="D65" s="144"/>
+      <c r="E65" s="145"/>
     </row>
     <row r="66" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B66" s="144"/>
-      <c r="C66" s="173" t="s">
+      <c r="B66" s="169"/>
+      <c r="C66" s="156" t="s">
         <v>209</v>
       </c>
-      <c r="D66" s="161"/>
-      <c r="E66" s="162"/>
+      <c r="D66" s="144"/>
+      <c r="E66" s="145"/>
     </row>
     <row r="67" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B67" s="144"/>
-      <c r="C67" s="173" t="s">
+      <c r="B67" s="169"/>
+      <c r="C67" s="156" t="s">
         <v>210</v>
       </c>
-      <c r="D67" s="161"/>
-      <c r="E67" s="162"/>
+      <c r="D67" s="144"/>
+      <c r="E67" s="145"/>
     </row>
     <row r="68" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B68" s="144"/>
-      <c r="C68" s="173" t="s">
+      <c r="B68" s="169"/>
+      <c r="C68" s="156" t="s">
         <v>208</v>
       </c>
-      <c r="D68" s="161"/>
-      <c r="E68" s="162"/>
+      <c r="D68" s="144"/>
+      <c r="E68" s="145"/>
     </row>
     <row r="69" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B69" s="144"/>
-      <c r="C69" s="173" t="s">
+      <c r="B69" s="169"/>
+      <c r="C69" s="156" t="s">
         <v>211</v>
       </c>
-      <c r="D69" s="161"/>
-      <c r="E69" s="162"/>
+      <c r="D69" s="144"/>
+      <c r="E69" s="145"/>
     </row>
     <row r="70" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B70" s="144"/>
-      <c r="C70" s="173"/>
-      <c r="D70" s="161"/>
-      <c r="E70" s="162"/>
+      <c r="B70" s="169"/>
+      <c r="C70" s="156"/>
+      <c r="D70" s="144"/>
+      <c r="E70" s="145"/>
     </row>
     <row r="71" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B71" s="144"/>
-      <c r="C71" s="173"/>
-      <c r="D71" s="161"/>
-      <c r="E71" s="162"/>
+      <c r="B71" s="169"/>
+      <c r="C71" s="156"/>
+      <c r="D71" s="144"/>
+      <c r="E71" s="145"/>
     </row>
     <row r="72" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B72" s="145"/>
-      <c r="C72" s="164"/>
-      <c r="D72" s="165"/>
-      <c r="E72" s="166"/>
+      <c r="B72" s="170"/>
+      <c r="C72" s="147"/>
+      <c r="D72" s="148"/>
+      <c r="E72" s="149"/>
     </row>
     <row r="73" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B73" s="157" t="s">
+      <c r="B73" s="167" t="s">
         <v>61</v>
       </c>
-      <c r="C73" s="173"/>
-      <c r="D73" s="181" t="s">
+      <c r="C73" s="156"/>
+      <c r="D73" s="164" t="s">
         <v>228</v>
       </c>
-      <c r="E73" s="181" t="s">
+      <c r="E73" s="164" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="74" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B74" s="144"/>
-      <c r="C74" s="173" t="s">
+      <c r="B74" s="169"/>
+      <c r="C74" s="156" t="s">
         <v>242</v>
       </c>
-      <c r="D74" s="174" t="s">
+      <c r="D74" s="157" t="s">
         <v>215</v>
       </c>
-      <c r="E74" s="175" t="s">
+      <c r="E74" s="158" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="75" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B75" s="144"/>
-      <c r="C75" s="163"/>
-      <c r="D75" s="174" t="s">
+      <c r="B75" s="169"/>
+      <c r="C75" s="146"/>
+      <c r="D75" s="157" t="s">
         <v>216</v>
       </c>
-      <c r="E75" s="175" t="s">
+      <c r="E75" s="158" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="76" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B76" s="144"/>
-      <c r="C76" s="163"/>
-      <c r="D76" s="161" t="s">
+      <c r="B76" s="169"/>
+      <c r="C76" s="146"/>
+      <c r="D76" s="144" t="s">
         <v>156</v>
       </c>
-      <c r="E76" s="175" t="s">
+      <c r="E76" s="158" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="77" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B77" s="144"/>
-      <c r="C77" s="163"/>
-      <c r="D77" s="161" t="s">
+      <c r="B77" s="169"/>
+      <c r="C77" s="146"/>
+      <c r="D77" s="144" t="s">
         <v>157</v>
       </c>
-      <c r="E77" s="175" t="s">
+      <c r="E77" s="158" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="78" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B78" s="144"/>
-      <c r="C78" s="163"/>
-      <c r="D78" s="174" t="s">
+      <c r="B78" s="169"/>
+      <c r="C78" s="146"/>
+      <c r="D78" s="157" t="s">
         <v>160</v>
       </c>
-      <c r="E78" s="175" t="s">
+      <c r="E78" s="158" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="79" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B79" s="144"/>
-      <c r="C79" s="163"/>
-      <c r="D79" s="174" t="s">
+      <c r="B79" s="169"/>
+      <c r="C79" s="146"/>
+      <c r="D79" s="157" t="s">
         <v>233</v>
       </c>
-      <c r="E79" s="175" t="s">
+      <c r="E79" s="158" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="80" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B80" s="144"/>
-      <c r="C80" s="163"/>
-      <c r="D80" s="174" t="s">
+      <c r="B80" s="169"/>
+      <c r="C80" s="146"/>
+      <c r="D80" s="157" t="s">
         <v>212</v>
       </c>
-      <c r="E80" s="175" t="s">
+      <c r="E80" s="158" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="81" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B81" s="144"/>
-      <c r="C81" s="163"/>
-      <c r="D81" s="174" t="s">
+      <c r="B81" s="169"/>
+      <c r="C81" s="146"/>
+      <c r="D81" s="157" t="s">
         <v>213</v>
       </c>
-      <c r="E81" s="175" t="s">
+      <c r="E81" s="158" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="82" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B82" s="144"/>
-      <c r="C82" s="163"/>
-      <c r="D82" s="174" t="s">
+      <c r="B82" s="169"/>
+      <c r="C82" s="146"/>
+      <c r="D82" s="157" t="s">
         <v>214</v>
       </c>
-      <c r="E82" s="175" t="s">
+      <c r="E82" s="158" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="83" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B83" s="144"/>
-      <c r="C83" s="173"/>
-      <c r="D83" s="174" t="s">
+      <c r="B83" s="169"/>
+      <c r="C83" s="156"/>
+      <c r="D83" s="157" t="s">
         <v>234</v>
       </c>
-      <c r="E83" s="175" t="s">
+      <c r="E83" s="158" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="84" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B84" s="144"/>
-      <c r="C84" s="173"/>
-      <c r="D84" s="174" t="s">
+      <c r="B84" s="169"/>
+      <c r="C84" s="156"/>
+      <c r="D84" s="157" t="s">
         <v>235</v>
       </c>
-      <c r="E84" s="175" t="s">
+      <c r="E84" s="158" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="85" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B85" s="144"/>
-      <c r="C85" s="163"/>
-      <c r="D85" s="174" t="s">
+      <c r="B85" s="169"/>
+      <c r="C85" s="146"/>
+      <c r="D85" s="157" t="s">
         <v>236</v>
       </c>
-      <c r="E85" s="175" t="s">
+      <c r="E85" s="158" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="86" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B86" s="144"/>
-      <c r="C86" s="163"/>
-      <c r="D86" s="174" t="s">
+      <c r="B86" s="169"/>
+      <c r="C86" s="146"/>
+      <c r="D86" s="157" t="s">
         <v>238</v>
       </c>
-      <c r="E86" s="175" t="s">
+      <c r="E86" s="158" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="87" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B87" s="144"/>
-      <c r="C87" s="163"/>
-      <c r="D87" s="174" t="s">
+      <c r="B87" s="169"/>
+      <c r="C87" s="146"/>
+      <c r="D87" s="157" t="s">
         <v>247</v>
       </c>
-      <c r="E87" s="175" t="s">
+      <c r="E87" s="158" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="88" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B88" s="144"/>
-      <c r="C88" s="163"/>
-      <c r="D88" s="174" t="s">
+      <c r="B88" s="169"/>
+      <c r="C88" s="146"/>
+      <c r="D88" s="157" t="s">
         <v>248</v>
       </c>
-      <c r="E88" s="175" t="s">
+      <c r="E88" s="158" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="89" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B89" s="145"/>
-      <c r="C89" s="164"/>
-      <c r="D89" s="165"/>
-      <c r="E89" s="166"/>
+      <c r="B89" s="170"/>
+      <c r="C89" s="147"/>
+      <c r="D89" s="148"/>
+      <c r="E89" s="149"/>
     </row>
     <row r="90" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B90" s="157" t="s">
+      <c r="B90" s="167" t="s">
         <v>62</v>
       </c>
-      <c r="C90" s="167"/>
-      <c r="D90" s="168"/>
-      <c r="E90" s="169"/>
+      <c r="C90" s="150"/>
+      <c r="D90" s="151"/>
+      <c r="E90" s="152"/>
     </row>
     <row r="91" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B91" s="144"/>
-      <c r="C91" s="173" t="s">
+      <c r="B91" s="169"/>
+      <c r="C91" s="156" t="s">
         <v>243</v>
       </c>
-      <c r="D91" s="174"/>
-      <c r="E91" s="162"/>
+      <c r="D91" s="157"/>
+      <c r="E91" s="145"/>
     </row>
     <row r="92" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B92" s="144"/>
-      <c r="C92" s="173" t="s">
+      <c r="B92" s="169"/>
+      <c r="C92" s="156" t="s">
         <v>244</v>
       </c>
-      <c r="D92" s="161"/>
-      <c r="E92" s="162"/>
+      <c r="D92" s="144"/>
+      <c r="E92" s="145"/>
     </row>
     <row r="93" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B93" s="144"/>
-      <c r="C93" s="163" t="s">
+      <c r="B93" s="169"/>
+      <c r="C93" s="146" t="s">
         <v>245</v>
       </c>
-      <c r="D93" s="161"/>
-      <c r="E93" s="162"/>
+      <c r="D93" s="144"/>
+      <c r="E93" s="145"/>
     </row>
     <row r="94" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B94" s="144"/>
-      <c r="C94" s="163"/>
-      <c r="D94" s="161"/>
-      <c r="E94" s="162"/>
+      <c r="B94" s="169"/>
+      <c r="C94" s="146"/>
+      <c r="D94" s="144"/>
+      <c r="E94" s="145"/>
     </row>
     <row r="95" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B95" s="144"/>
-      <c r="C95" s="163"/>
-      <c r="D95" s="161"/>
-      <c r="E95" s="162"/>
+      <c r="B95" s="169"/>
+      <c r="C95" s="146"/>
+      <c r="D95" s="144"/>
+      <c r="E95" s="145"/>
     </row>
     <row r="96" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B96" s="144"/>
-      <c r="C96" s="163"/>
-      <c r="D96" s="161"/>
-      <c r="E96" s="162"/>
+      <c r="B96" s="169"/>
+      <c r="C96" s="146"/>
+      <c r="D96" s="144"/>
+      <c r="E96" s="145"/>
     </row>
     <row r="97" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B97" s="144"/>
-      <c r="C97" s="163"/>
-      <c r="D97" s="161"/>
-      <c r="E97" s="162"/>
+      <c r="B97" s="169"/>
+      <c r="C97" s="146"/>
+      <c r="D97" s="144"/>
+      <c r="E97" s="145"/>
     </row>
     <row r="98" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B98" s="144"/>
-      <c r="C98" s="163"/>
-      <c r="D98" s="161"/>
-      <c r="E98" s="162"/>
+      <c r="B98" s="169"/>
+      <c r="C98" s="146"/>
+      <c r="D98" s="144"/>
+      <c r="E98" s="145"/>
     </row>
     <row r="99" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B99" s="145"/>
-      <c r="C99" s="170"/>
-      <c r="D99" s="171"/>
-      <c r="E99" s="172"/>
+      <c r="B99" s="170"/>
+      <c r="C99" s="153"/>
+      <c r="D99" s="154"/>
+      <c r="E99" s="155"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4016,8 +4432,8 @@
   </sheetPr>
   <dimension ref="B2:I28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
@@ -4047,26 +4463,26 @@
     </row>
     <row r="3" spans="2:9" ht="56.25" customHeight="1">
       <c r="B3" s="80"/>
-      <c r="C3" s="146" t="s">
+      <c r="C3" s="171" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="146"/>
-      <c r="E3" s="146"/>
-      <c r="F3" s="146"/>
-      <c r="G3" s="146"/>
-      <c r="H3" s="146"/>
-      <c r="I3" s="146"/>
+      <c r="D3" s="171"/>
+      <c r="E3" s="171"/>
+      <c r="F3" s="171"/>
+      <c r="G3" s="171"/>
+      <c r="H3" s="171"/>
+      <c r="I3" s="171"/>
     </row>
     <row r="4" spans="2:9" ht="30.75" customHeight="1">
       <c r="B4" s="81"/>
-      <c r="C4" s="147" t="s">
+      <c r="C4" s="172" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="147"/>
-      <c r="E4" s="147"/>
-      <c r="F4" s="147"/>
-      <c r="G4" s="143"/>
-      <c r="H4" s="143"/>
+      <c r="D4" s="172"/>
+      <c r="E4" s="172"/>
+      <c r="F4" s="172"/>
+      <c r="G4" s="166"/>
+      <c r="H4" s="166"/>
       <c r="I4" s="81"/>
     </row>
     <row r="5" spans="2:9" ht="21" customHeight="1">
@@ -4265,246 +4681,716 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B2:I28"/>
+  <dimension ref="B1:G88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
-    <col min="5" max="6" width="22.5703125" customWidth="1"/>
-    <col min="7" max="7" width="44.42578125" customWidth="1"/>
-    <col min="8" max="8" width="49.5703125" customWidth="1"/>
-    <col min="9" max="9" width="46.140625" customWidth="1"/>
-    <col min="10" max="11" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="225" customWidth="1"/>
+    <col min="3" max="3" width="49.28515625" customWidth="1"/>
+    <col min="4" max="4" width="44.42578125" customWidth="1"/>
+    <col min="5" max="6" width="49.5703125" customWidth="1"/>
+    <col min="7" max="7" width="49.28515625" customWidth="1"/>
+    <col min="8" max="9" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B2" s="80"/>
-      <c r="C2" s="18" t="s">
+    <row r="1" spans="2:7" ht="15.75" customHeight="1" thickBot="1"/>
+    <row r="2" spans="2:7" ht="20.25" customHeight="1" thickBot="1">
+      <c r="B2" s="226"/>
+      <c r="C2" s="182" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
+      <c r="D2" s="183"/>
+      <c r="E2" s="184"/>
+      <c r="F2" s="184"/>
       <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-    </row>
-    <row r="3" spans="2:9" ht="56.25" customHeight="1">
-      <c r="B3" s="80"/>
-      <c r="C3" s="146" t="s">
+    </row>
+    <row r="3" spans="2:7" s="189" customFormat="1" ht="56.25" customHeight="1">
+      <c r="B3" s="227"/>
+      <c r="C3" s="186" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="146"/>
-      <c r="E3" s="146"/>
-      <c r="F3" s="146"/>
-      <c r="G3" s="146"/>
-      <c r="H3" s="146"/>
-      <c r="I3" s="146"/>
-    </row>
-    <row r="4" spans="2:9" ht="30.75" customHeight="1">
-      <c r="B4" s="81"/>
-      <c r="C4" s="147" t="s">
+      <c r="D3" s="187"/>
+      <c r="E3" s="188"/>
+      <c r="G3" s="185"/>
+    </row>
+    <row r="4" spans="2:7" s="189" customFormat="1" ht="30.75" customHeight="1">
+      <c r="B4" s="227"/>
+      <c r="C4" s="190" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="147"/>
-      <c r="E4" s="147"/>
-      <c r="F4" s="147"/>
-      <c r="G4" s="143"/>
-      <c r="H4" s="143"/>
-      <c r="I4" s="81"/>
-    </row>
-    <row r="5" spans="2:9" ht="21" customHeight="1">
-      <c r="B5" s="80"/>
-      <c r="C5" s="16" t="s">
+      <c r="D4" s="187"/>
+      <c r="E4" s="188"/>
+    </row>
+    <row r="5" spans="2:7" ht="21" customHeight="1">
+      <c r="B5" s="226"/>
+      <c r="C5" s="191" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="80"/>
-    </row>
-    <row r="6" spans="2:9" ht="21" customHeight="1">
-      <c r="B6" s="81"/>
-      <c r="C6" s="17" t="s">
+      <c r="D5" s="80"/>
+      <c r="E5" s="192"/>
+      <c r="F5" s="192"/>
+    </row>
+    <row r="6" spans="2:7" ht="21" customHeight="1" thickBot="1">
+      <c r="B6" s="228"/>
+      <c r="C6" s="193" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
-      <c r="I6" s="81"/>
-    </row>
-    <row r="7" spans="2:9" ht="18" customHeight="1">
-      <c r="B7" s="81"/>
+      <c r="D6" s="194"/>
+      <c r="E6" s="195"/>
+      <c r="F6" s="195"/>
+    </row>
+    <row r="7" spans="2:7" ht="18" customHeight="1">
+      <c r="B7" s="228"/>
       <c r="C7" s="82"/>
       <c r="D7" s="82"/>
       <c r="E7" s="82"/>
       <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="81"/>
-    </row>
-    <row r="8" spans="2:9" ht="18" customHeight="1">
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="81"/>
-      <c r="I8" s="18"/>
-    </row>
-    <row r="9" spans="2:9" ht="19.5" customHeight="1">
-      <c r="B9" s="19" t="s">
+    </row>
+    <row r="8" spans="2:7" ht="18" customHeight="1">
+      <c r="B8" s="228"/>
+      <c r="C8" s="196" t="s">
+        <v>249</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+    </row>
+    <row r="9" spans="2:7" ht="19.5" customHeight="1">
+      <c r="B9" s="228"/>
+      <c r="C9" s="197" t="s">
+        <v>250</v>
+      </c>
+      <c r="D9" s="198"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="82"/>
+    </row>
+    <row r="10" spans="2:7" ht="18" customHeight="1">
+      <c r="B10" s="18"/>
+      <c r="C10" s="199" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="200"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
+    </row>
+    <row r="11" spans="2:7" ht="18" customHeight="1" thickBot="1">
+      <c r="B11" s="18"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
+    </row>
+    <row r="12" spans="2:7" ht="18" customHeight="1">
+      <c r="B12" s="201" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19" t="s">
+      <c r="C12" s="202" t="s">
+        <v>251</v>
+      </c>
+      <c r="D12" s="203" t="s">
         <v>70</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="E12" s="204" t="s">
         <v>71</v>
       </c>
-      <c r="I9" s="19"/>
-    </row>
-    <row r="10" spans="2:9" ht="18" customHeight="1">
-      <c r="B10" s="81"/>
-      <c r="C10" s="82"/>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="81"/>
-      <c r="H10" s="81"/>
-      <c r="I10" s="81"/>
-    </row>
-    <row r="11" spans="2:9" ht="18" customHeight="1">
-      <c r="B11" s="13" t="s">
+      <c r="F12" s="204" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="18" customHeight="1">
+      <c r="B13" s="222" t="s">
+        <v>252</v>
+      </c>
+      <c r="C13" s="219"/>
+      <c r="D13" s="220"/>
+      <c r="E13" s="221"/>
+      <c r="F13" s="221"/>
+    </row>
+    <row r="14" spans="2:7" ht="48" thickBot="1">
+      <c r="B14" s="223" t="s">
+        <v>261</v>
+      </c>
+      <c r="C14" s="205" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="F11" s="137" t="s">
-        <v>75</v>
-      </c>
-      <c r="G11" s="138" t="s">
+      <c r="D14" s="81"/>
+      <c r="E14" s="206"/>
+      <c r="F14" s="206"/>
+      <c r="G14" s="81"/>
+    </row>
+    <row r="15" spans="2:7" ht="15.75" customHeight="1" thickTop="1">
+      <c r="B15" s="229"/>
+      <c r="C15" s="208"/>
+      <c r="D15" s="209" t="s">
         <v>76</v>
       </c>
-      <c r="H11" s="139" t="s">
-        <v>77</v>
-      </c>
-      <c r="I11" s="20" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" ht="18" customHeight="1">
-      <c r="B12" s="81"/>
-      <c r="C12" s="82"/>
-      <c r="D12" s="82"/>
-      <c r="E12" s="82"/>
-      <c r="F12" s="82"/>
-      <c r="G12" s="140"/>
-      <c r="H12" s="112"/>
-      <c r="I12" s="81" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" ht="18" customHeight="1">
-      <c r="B13" s="81"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="105"/>
-      <c r="H13" s="111"/>
-      <c r="I13" s="81" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" ht="15.75" customHeight="1">
-      <c r="G14" s="106"/>
-      <c r="H14" s="107"/>
-    </row>
-    <row r="15" spans="2:9" ht="15.75" customHeight="1">
-      <c r="G15" s="106"/>
-      <c r="H15" s="107"/>
-    </row>
-    <row r="16" spans="2:9" ht="15.75" customHeight="1">
-      <c r="G16" s="106"/>
-      <c r="H16" s="107"/>
-    </row>
-    <row r="17" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G17" s="106"/>
-      <c r="H17" s="107"/>
-    </row>
-    <row r="18" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G18" s="106"/>
-      <c r="H18" s="107"/>
-    </row>
-    <row r="19" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G19" s="106"/>
-      <c r="H19" s="107"/>
-    </row>
-    <row r="20" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G20" s="106"/>
-      <c r="H20" s="107"/>
-    </row>
-    <row r="21" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G21" s="106"/>
-      <c r="H21" s="107"/>
-    </row>
-    <row r="22" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G22" s="106"/>
-      <c r="H22" s="107"/>
-    </row>
-    <row r="23" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G23" s="106"/>
-      <c r="H23" s="107"/>
-    </row>
-    <row r="24" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G24" s="106"/>
-      <c r="H24" s="107"/>
-    </row>
-    <row r="25" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G25" s="106"/>
-      <c r="H25" s="107"/>
-    </row>
-    <row r="26" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G26" s="106"/>
-      <c r="H26" s="107"/>
-    </row>
-    <row r="27" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G27" s="106"/>
-      <c r="H27" s="107"/>
-    </row>
-    <row r="28" spans="7:8" ht="18" customHeight="1">
-      <c r="G28" s="114" t="s">
-        <v>81</v>
-      </c>
-      <c r="H28" s="110"/>
+      <c r="E15" s="233" t="s">
+        <v>280</v>
+      </c>
+      <c r="F15" s="233" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B16" s="230" t="s">
+        <v>255</v>
+      </c>
+      <c r="C16" s="224" t="s">
+        <v>253</v>
+      </c>
+      <c r="D16" s="211"/>
+      <c r="E16" s="212"/>
+      <c r="F16" s="212"/>
+    </row>
+    <row r="17" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B17" s="229"/>
+      <c r="C17" s="207"/>
+      <c r="D17" s="211"/>
+      <c r="E17" s="212"/>
+      <c r="F17" s="212"/>
+    </row>
+    <row r="18" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B18" s="230" t="s">
+        <v>255</v>
+      </c>
+      <c r="C18" s="224" t="s">
+        <v>254</v>
+      </c>
+      <c r="D18" s="214"/>
+      <c r="E18" s="215"/>
+      <c r="F18" s="215"/>
+    </row>
+    <row r="19" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B19" s="229"/>
+      <c r="C19" s="207"/>
+      <c r="D19" s="214"/>
+      <c r="E19" s="215"/>
+      <c r="F19" s="215"/>
+    </row>
+    <row r="20" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B20" s="230" t="s">
+        <v>255</v>
+      </c>
+      <c r="C20" s="224" t="s">
+        <v>256</v>
+      </c>
+      <c r="D20" s="214"/>
+      <c r="E20" s="215"/>
+      <c r="F20" s="215"/>
+    </row>
+    <row r="21" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B21" s="229"/>
+      <c r="C21" s="207"/>
+      <c r="D21" s="214"/>
+      <c r="E21" s="215"/>
+      <c r="F21" s="215"/>
+    </row>
+    <row r="22" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B22" s="230" t="s">
+        <v>255</v>
+      </c>
+      <c r="C22" s="224" t="s">
+        <v>257</v>
+      </c>
+      <c r="D22" s="214"/>
+      <c r="E22" s="215"/>
+      <c r="F22" s="215"/>
+    </row>
+    <row r="23" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B23" s="229"/>
+      <c r="C23" s="207"/>
+      <c r="D23" s="214"/>
+      <c r="E23" s="215"/>
+      <c r="F23" s="215"/>
+    </row>
+    <row r="24" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B24" s="230" t="s">
+        <v>255</v>
+      </c>
+      <c r="C24" s="224" t="s">
+        <v>258</v>
+      </c>
+      <c r="D24" s="214"/>
+      <c r="E24" s="215"/>
+      <c r="F24" s="215"/>
+    </row>
+    <row r="25" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B25" s="229"/>
+      <c r="C25" s="207"/>
+      <c r="D25" s="214"/>
+      <c r="E25" s="215"/>
+      <c r="F25" s="215"/>
+    </row>
+    <row r="26" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B26" s="230" t="s">
+        <v>255</v>
+      </c>
+      <c r="C26" s="224" t="s">
+        <v>259</v>
+      </c>
+      <c r="D26" s="214"/>
+      <c r="E26" s="215"/>
+      <c r="F26" s="215"/>
+    </row>
+    <row r="27" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B27" s="229"/>
+      <c r="C27" s="207"/>
+      <c r="D27" s="214"/>
+      <c r="E27" s="215"/>
+      <c r="F27" s="215"/>
+    </row>
+    <row r="28" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B28" s="230" t="s">
+        <v>255</v>
+      </c>
+      <c r="C28" s="224" t="s">
+        <v>260</v>
+      </c>
+      <c r="D28" s="214"/>
+      <c r="E28" s="215"/>
+      <c r="F28" s="215"/>
+    </row>
+    <row r="29" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B29" s="229"/>
+      <c r="C29" s="207"/>
+      <c r="D29" s="214"/>
+      <c r="E29" s="215"/>
+      <c r="F29" s="215"/>
+    </row>
+    <row r="30" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B30" s="230" t="s">
+        <v>255</v>
+      </c>
+      <c r="C30" s="224" t="s">
+        <v>262</v>
+      </c>
+      <c r="D30" s="214"/>
+      <c r="E30" s="215"/>
+      <c r="F30" s="215"/>
+    </row>
+    <row r="31" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B31" s="229"/>
+      <c r="C31" s="207"/>
+      <c r="D31" s="214"/>
+      <c r="E31" s="215"/>
+      <c r="F31" s="215"/>
+    </row>
+    <row r="32" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B32" s="230" t="s">
+        <v>255</v>
+      </c>
+      <c r="C32" s="224" t="s">
+        <v>263</v>
+      </c>
+      <c r="D32" s="214"/>
+      <c r="E32" s="215"/>
+      <c r="F32" s="215"/>
+    </row>
+    <row r="33" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B33" s="229"/>
+      <c r="C33" s="207"/>
+      <c r="D33" s="214"/>
+      <c r="E33" s="215"/>
+      <c r="F33" s="215"/>
+    </row>
+    <row r="34" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B34" s="230" t="s">
+        <v>255</v>
+      </c>
+      <c r="C34" s="224" t="s">
+        <v>264</v>
+      </c>
+      <c r="D34" s="214"/>
+      <c r="E34" s="215"/>
+      <c r="F34" s="215"/>
+    </row>
+    <row r="35" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B35" s="229"/>
+      <c r="C35" s="207"/>
+      <c r="D35" s="214"/>
+      <c r="E35" s="215"/>
+      <c r="F35" s="215"/>
+    </row>
+    <row r="36" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B36" s="230" t="s">
+        <v>265</v>
+      </c>
+      <c r="C36" s="224" t="s">
+        <v>266</v>
+      </c>
+      <c r="D36" s="214"/>
+      <c r="E36" s="215"/>
+      <c r="F36" s="215"/>
+    </row>
+    <row r="37" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B37" s="229"/>
+      <c r="C37" s="207"/>
+      <c r="D37" s="214"/>
+      <c r="E37" s="215"/>
+      <c r="F37" s="215"/>
+    </row>
+    <row r="38" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B38" s="230" t="s">
+        <v>265</v>
+      </c>
+      <c r="C38" s="224" t="s">
+        <v>267</v>
+      </c>
+      <c r="D38" s="214"/>
+      <c r="E38" s="215"/>
+      <c r="F38" s="215"/>
+    </row>
+    <row r="39" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B39" s="229"/>
+      <c r="C39" s="207"/>
+      <c r="D39" s="214"/>
+      <c r="E39" s="215"/>
+      <c r="F39" s="215"/>
+    </row>
+    <row r="40" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B40" s="230" t="s">
+        <v>265</v>
+      </c>
+      <c r="C40" s="224" t="s">
+        <v>268</v>
+      </c>
+      <c r="D40" s="214"/>
+      <c r="E40" s="215"/>
+      <c r="F40" s="215"/>
+    </row>
+    <row r="41" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B41" s="229"/>
+      <c r="C41" s="207"/>
+      <c r="D41" s="214"/>
+      <c r="E41" s="215"/>
+      <c r="F41" s="215"/>
+    </row>
+    <row r="42" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B42" s="230" t="s">
+        <v>269</v>
+      </c>
+      <c r="C42" s="224" t="s">
+        <v>270</v>
+      </c>
+      <c r="D42" s="214"/>
+      <c r="E42" s="215"/>
+      <c r="F42" s="215"/>
+    </row>
+    <row r="43" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B43" s="229"/>
+      <c r="C43" s="207"/>
+      <c r="D43" s="214"/>
+      <c r="E43" s="215"/>
+      <c r="F43" s="215"/>
+    </row>
+    <row r="44" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B44" s="230" t="s">
+        <v>269</v>
+      </c>
+      <c r="C44" s="224" t="s">
+        <v>271</v>
+      </c>
+      <c r="D44" s="214"/>
+      <c r="E44" s="215"/>
+      <c r="F44" s="215"/>
+    </row>
+    <row r="45" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B45" s="229"/>
+      <c r="C45" s="207"/>
+      <c r="D45" s="214"/>
+      <c r="E45" s="215"/>
+      <c r="F45" s="215"/>
+    </row>
+    <row r="46" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B46" s="230" t="s">
+        <v>269</v>
+      </c>
+      <c r="C46" s="224" t="s">
+        <v>272</v>
+      </c>
+      <c r="D46" s="214"/>
+      <c r="E46" s="215"/>
+      <c r="F46" s="215"/>
+    </row>
+    <row r="47" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B47" s="229"/>
+      <c r="C47" s="207"/>
+      <c r="D47" s="214"/>
+      <c r="E47" s="215"/>
+      <c r="F47" s="215"/>
+    </row>
+    <row r="48" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B48" s="230" t="s">
+        <v>269</v>
+      </c>
+      <c r="C48" s="224" t="s">
+        <v>273</v>
+      </c>
+      <c r="D48" s="214"/>
+      <c r="E48" s="215"/>
+      <c r="F48" s="215"/>
+    </row>
+    <row r="49" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B49" s="229"/>
+      <c r="C49" s="207"/>
+      <c r="D49" s="214"/>
+      <c r="E49" s="215"/>
+      <c r="F49" s="215"/>
+    </row>
+    <row r="50" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B50" s="230" t="s">
+        <v>269</v>
+      </c>
+      <c r="C50" s="224" t="s">
+        <v>274</v>
+      </c>
+      <c r="D50" s="214"/>
+      <c r="E50" s="215"/>
+      <c r="F50" s="215"/>
+    </row>
+    <row r="51" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B51" s="229"/>
+      <c r="C51" s="207"/>
+      <c r="D51" s="214"/>
+      <c r="E51" s="215"/>
+      <c r="F51" s="215"/>
+    </row>
+    <row r="52" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B52" s="230" t="s">
+        <v>269</v>
+      </c>
+      <c r="C52" s="224" t="s">
+        <v>275</v>
+      </c>
+      <c r="D52" s="214"/>
+      <c r="E52" s="215"/>
+      <c r="F52" s="215"/>
+    </row>
+    <row r="53" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B53" s="229"/>
+      <c r="C53" s="207"/>
+      <c r="D53" s="214"/>
+      <c r="E53" s="215"/>
+      <c r="F53" s="215"/>
+    </row>
+    <row r="54" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B54" s="230" t="s">
+        <v>269</v>
+      </c>
+      <c r="C54" s="224" t="s">
+        <v>278</v>
+      </c>
+      <c r="D54" s="214"/>
+      <c r="E54" s="215"/>
+      <c r="F54" s="215"/>
+    </row>
+    <row r="55" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B55" s="229"/>
+      <c r="C55" s="207"/>
+      <c r="D55" s="214"/>
+      <c r="E55" s="215"/>
+      <c r="F55" s="215"/>
+    </row>
+    <row r="56" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B56" s="230" t="s">
+        <v>269</v>
+      </c>
+      <c r="C56" s="224" t="s">
+        <v>276</v>
+      </c>
+      <c r="D56" s="214"/>
+      <c r="E56" s="215"/>
+      <c r="F56" s="215"/>
+    </row>
+    <row r="57" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B57" s="229"/>
+      <c r="C57" s="207"/>
+      <c r="D57" s="214"/>
+      <c r="E57" s="215"/>
+      <c r="F57" s="215"/>
+    </row>
+    <row r="58" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B58" s="230" t="s">
+        <v>269</v>
+      </c>
+      <c r="C58" s="224" t="s">
+        <v>277</v>
+      </c>
+      <c r="D58" s="214"/>
+      <c r="E58" s="215"/>
+      <c r="F58" s="215"/>
+    </row>
+    <row r="59" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B59" s="229"/>
+      <c r="C59" s="207"/>
+      <c r="D59" s="214"/>
+      <c r="E59" s="215"/>
+      <c r="F59" s="215"/>
+    </row>
+    <row r="60" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B60" s="230" t="s">
+        <v>269</v>
+      </c>
+      <c r="C60" s="224" t="s">
+        <v>279</v>
+      </c>
+      <c r="D60" s="214"/>
+      <c r="E60" s="215"/>
+      <c r="F60" s="215"/>
+    </row>
+    <row r="61" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B61" s="229"/>
+      <c r="C61" s="207"/>
+      <c r="D61" s="214"/>
+      <c r="E61" s="215"/>
+      <c r="F61" s="215"/>
+    </row>
+    <row r="62" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B62" s="229"/>
+      <c r="C62" s="207"/>
+      <c r="D62" s="214"/>
+      <c r="E62" s="215"/>
+      <c r="F62" s="215"/>
+    </row>
+    <row r="63" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B63" s="229"/>
+      <c r="C63" s="207"/>
+      <c r="D63" s="214"/>
+      <c r="E63" s="215"/>
+      <c r="F63" s="215"/>
+    </row>
+    <row r="64" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B64" s="229"/>
+      <c r="C64" s="207"/>
+      <c r="D64" s="214"/>
+      <c r="E64" s="215"/>
+      <c r="F64" s="215"/>
+    </row>
+    <row r="65" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B65" s="229"/>
+      <c r="C65" s="207"/>
+      <c r="D65" s="214"/>
+      <c r="E65" s="215"/>
+      <c r="F65" s="215"/>
+    </row>
+    <row r="66" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B66" s="229"/>
+      <c r="C66" s="207"/>
+      <c r="D66" s="214"/>
+      <c r="E66" s="215"/>
+      <c r="F66" s="215"/>
+    </row>
+    <row r="67" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B67" s="229"/>
+      <c r="C67" s="207"/>
+      <c r="D67" s="214"/>
+      <c r="E67" s="215"/>
+      <c r="F67" s="215"/>
+    </row>
+    <row r="68" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B68" s="229"/>
+      <c r="C68" s="207"/>
+      <c r="D68" s="214"/>
+      <c r="E68" s="215"/>
+      <c r="F68" s="215"/>
+    </row>
+    <row r="69" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B69" s="229"/>
+      <c r="C69" s="207"/>
+      <c r="D69" s="214"/>
+      <c r="E69" s="215"/>
+      <c r="F69" s="215"/>
+    </row>
+    <row r="70" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B70" s="229"/>
+      <c r="C70" s="207"/>
+      <c r="D70" s="214"/>
+      <c r="E70" s="215"/>
+      <c r="F70" s="215"/>
+    </row>
+    <row r="71" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B71" s="229"/>
+      <c r="C71" s="207"/>
+      <c r="D71" s="214"/>
+      <c r="E71" s="215"/>
+      <c r="F71" s="215"/>
+    </row>
+    <row r="72" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B72" s="231"/>
+      <c r="C72" s="210"/>
+      <c r="D72" s="211"/>
+      <c r="E72" s="212"/>
+      <c r="F72" s="212"/>
+    </row>
+    <row r="73" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B73" s="231"/>
+      <c r="C73" s="213"/>
+      <c r="D73" s="211"/>
+      <c r="E73" s="212"/>
+      <c r="F73" s="212"/>
+    </row>
+    <row r="74" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B74" s="229"/>
+      <c r="C74" s="207"/>
+      <c r="D74" s="214"/>
+      <c r="E74" s="215"/>
+      <c r="F74" s="215"/>
+    </row>
+    <row r="75" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B75" s="229"/>
+      <c r="C75" s="207"/>
+      <c r="D75" s="214"/>
+      <c r="E75" s="215"/>
+      <c r="F75" s="215"/>
+    </row>
+    <row r="76" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B76" s="229"/>
+      <c r="C76" s="207"/>
+      <c r="D76" s="214"/>
+      <c r="E76" s="215"/>
+      <c r="F76" s="215"/>
+    </row>
+    <row r="77" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B77" s="229"/>
+      <c r="C77" s="207"/>
+      <c r="D77" s="214"/>
+      <c r="E77" s="215"/>
+      <c r="F77" s="215"/>
+    </row>
+    <row r="78" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B78" s="229"/>
+      <c r="C78" s="207"/>
+      <c r="D78" s="214"/>
+      <c r="E78" s="215"/>
+      <c r="F78" s="215"/>
+    </row>
+    <row r="79" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B79" s="229"/>
+      <c r="C79" s="207"/>
+      <c r="D79" s="214"/>
+      <c r="E79" s="215"/>
+      <c r="F79" s="215"/>
+    </row>
+    <row r="80" spans="2:6" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B80" s="232"/>
+      <c r="C80" s="216"/>
+      <c r="D80" s="217"/>
+      <c r="E80" s="218"/>
+      <c r="F80" s="218"/>
+    </row>
+    <row r="85" spans="4:4" ht="18" customHeight="1"/>
+    <row r="88" spans="4:4" ht="15.75" customHeight="1">
+      <c r="D88" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4696,13 +5582,13 @@
       <c r="J11" s="82"/>
       <c r="K11" s="82"/>
       <c r="L11" s="82"/>
-      <c r="M11" s="149"/>
-      <c r="N11" s="143"/>
-      <c r="O11" s="143"/>
+      <c r="M11" s="174"/>
+      <c r="N11" s="166"/>
+      <c r="O11" s="166"/>
       <c r="P11" s="82"/>
       <c r="Q11" s="82"/>
-      <c r="R11" s="149"/>
-      <c r="S11" s="150"/>
+      <c r="R11" s="174"/>
+      <c r="S11" s="175"/>
     </row>
     <row r="12" spans="7:19" ht="15">
       <c r="G12" s="26"/>
@@ -4912,9 +5798,9 @@
       <c r="W23" s="82"/>
     </row>
     <row r="24" spans="7:23" ht="15">
-      <c r="G24" s="148"/>
-      <c r="H24" s="143"/>
-      <c r="I24" s="143"/>
+      <c r="G24" s="173"/>
+      <c r="H24" s="166"/>
+      <c r="I24" s="166"/>
       <c r="J24" s="82"/>
       <c r="K24" s="82"/>
       <c r="L24" s="82"/>
@@ -4950,9 +5836,9 @@
       <c r="W25" s="82"/>
     </row>
     <row r="26" spans="7:23" ht="15">
-      <c r="G26" s="148"/>
-      <c r="H26" s="143"/>
-      <c r="I26" s="143"/>
+      <c r="G26" s="173"/>
+      <c r="H26" s="166"/>
+      <c r="I26" s="166"/>
       <c r="J26" s="82"/>
       <c r="K26" s="82"/>
       <c r="L26" s="82"/>
@@ -4997,14 +5883,14 @@
       <c r="M28" s="82"/>
       <c r="N28" s="82"/>
       <c r="O28" s="82"/>
-      <c r="P28" s="148"/>
-      <c r="Q28" s="143"/>
-      <c r="R28" s="143"/>
+      <c r="P28" s="173"/>
+      <c r="Q28" s="166"/>
+      <c r="R28" s="166"/>
       <c r="S28" s="82"/>
-      <c r="T28" s="148"/>
-      <c r="U28" s="143"/>
-      <c r="V28" s="143"/>
-      <c r="W28" s="143"/>
+      <c r="T28" s="173"/>
+      <c r="U28" s="166"/>
+      <c r="V28" s="166"/>
+      <c r="W28" s="166"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -5054,16 +5940,16 @@
     </row>
     <row r="3" spans="2:10" ht="84" customHeight="1">
       <c r="B3" s="81"/>
-      <c r="C3" s="146" t="s">
+      <c r="C3" s="171" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="146"/>
-      <c r="E3" s="146"/>
-      <c r="F3" s="146"/>
-      <c r="G3" s="146"/>
-      <c r="H3" s="146"/>
-      <c r="I3" s="146"/>
-      <c r="J3" s="146"/>
+      <c r="D3" s="171"/>
+      <c r="E3" s="171"/>
+      <c r="F3" s="171"/>
+      <c r="G3" s="171"/>
+      <c r="H3" s="171"/>
+      <c r="I3" s="171"/>
+      <c r="J3" s="171"/>
     </row>
     <row r="4" spans="2:10" ht="12.75" customHeight="1">
       <c r="B4" s="102"/>
@@ -5247,32 +6133,32 @@
       </c>
     </row>
     <row r="3" spans="2:11" ht="17.25" customHeight="1">
-      <c r="C3" s="154" t="s">
+      <c r="C3" s="179" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="154"/>
-      <c r="E3" s="154"/>
-      <c r="F3" s="154"/>
-      <c r="G3" s="154"/>
-      <c r="H3" s="154"/>
-      <c r="I3" s="154"/>
-      <c r="J3" s="154"/>
-      <c r="K3" s="154"/>
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="179"/>
+      <c r="H3" s="179"/>
+      <c r="I3" s="179"/>
+      <c r="J3" s="179"/>
+      <c r="K3" s="179"/>
     </row>
     <row r="4" spans="2:11" ht="15" customHeight="1">
       <c r="C4" s="94"/>
     </row>
     <row r="5" spans="2:11" ht="12.75">
-      <c r="G5" s="152" t="s">
+      <c r="G5" s="177" t="s">
         <v>108</v>
       </c>
-      <c r="H5" s="153"/>
+      <c r="H5" s="178"/>
     </row>
     <row r="6" spans="2:11" ht="18.75" customHeight="1">
-      <c r="C6" s="151" t="s">
+      <c r="C6" s="176" t="s">
         <v>109</v>
       </c>
-      <c r="D6" s="151"/>
+      <c r="D6" s="176"/>
       <c r="G6" s="83" t="s">
         <v>110</v>
       </c>
@@ -5382,7 +6268,7 @@
   <dimension ref="B1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D11"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
@@ -5400,33 +6286,33 @@
     <row r="1" spans="2:8" ht="57" customHeight="1">
       <c r="B1" s="85"/>
       <c r="C1" s="86"/>
-      <c r="D1" s="155" t="s">
+      <c r="D1" s="180" t="s">
         <v>122</v>
       </c>
-      <c r="E1" s="143"/>
-      <c r="F1" s="143"/>
-      <c r="G1" s="143"/>
-      <c r="H1" s="143"/>
+      <c r="E1" s="166"/>
+      <c r="F1" s="166"/>
+      <c r="G1" s="166"/>
+      <c r="H1" s="166"/>
     </row>
     <row r="2" spans="2:8" ht="12.75" customHeight="1">
       <c r="B2" s="85"/>
       <c r="C2" s="86"/>
-      <c r="D2" s="153" t="s">
+      <c r="D2" s="178" t="s">
         <v>123</v>
       </c>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
-      <c r="G2" s="153"/>
-      <c r="H2" s="153"/>
+      <c r="E2" s="178"/>
+      <c r="F2" s="178"/>
+      <c r="G2" s="178"/>
+      <c r="H2" s="178"/>
     </row>
     <row r="3" spans="2:8" ht="12.75" customHeight="1">
       <c r="B3" s="85"/>
       <c r="C3" s="86"/>
-      <c r="D3" s="153"/>
-      <c r="E3" s="153"/>
-      <c r="F3" s="153"/>
-      <c r="G3" s="153"/>
-      <c r="H3" s="153"/>
+      <c r="D3" s="178"/>
+      <c r="E3" s="178"/>
+      <c r="F3" s="178"/>
+      <c r="G3" s="178"/>
+      <c r="H3" s="178"/>
     </row>
     <row r="4" spans="2:8" ht="12.75" customHeight="1">
       <c r="B4" s="39" t="s">
@@ -5508,7 +6394,7 @@
   <dimension ref="B2:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
@@ -5549,12 +6435,12 @@
       <c r="E3" s="43"/>
       <c r="F3" s="43"/>
       <c r="G3" s="43"/>
-      <c r="H3" s="156"/>
-      <c r="I3" s="143"/>
-      <c r="J3" s="143"/>
-      <c r="K3" s="143"/>
-      <c r="L3" s="143"/>
-      <c r="M3" s="143"/>
+      <c r="H3" s="181"/>
+      <c r="I3" s="166"/>
+      <c r="J3" s="166"/>
+      <c r="K3" s="166"/>
+      <c r="L3" s="166"/>
+      <c r="M3" s="166"/>
     </row>
     <row r="4" spans="2:13" ht="21.75" customHeight="1">
       <c r="B4" s="74"/>

</xml_diff>

<commit_message>
add : cas d'usage
</commit_message>
<xml_diff>
--- a/doc/chiffrier_sim_vie.xlsx
+++ b/doc/chiffrier_sim_vie.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\travail\sim_vie-420-C41-IN-\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\travail\sim_vie\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203274B2-E6AE-4AFE-A266-DD096DD4D582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250F98E1-2207-4220-B0A4-402FE99F1480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="377">
   <si>
     <t>Chiffrier de documentation de projets</t>
   </si>
@@ -1151,15 +1151,6 @@
     <t>Modification de nuages de pression</t>
   </si>
   <si>
-    <t>Changement de rapport nourriture / organisme</t>
-  </si>
-  <si>
-    <t>Changement de rapport terre / eau</t>
-  </si>
-  <si>
-    <t>Changement de la durée des cycles</t>
-  </si>
-  <si>
     <t>(usager, environnement, organisme)</t>
   </si>
   <si>
@@ -1175,12 +1166,6 @@
     <t>environnement</t>
   </si>
   <si>
-    <t>Déplacement des nuages de pression</t>
-  </si>
-  <si>
-    <t>Génération de nourriture</t>
-  </si>
-  <si>
     <t>Changement de cycle</t>
   </si>
   <si>
@@ -1193,9 +1178,6 @@
     <t>Boire</t>
   </si>
   <si>
-    <t>Déféquer</t>
-  </si>
-  <si>
     <t>Mourir</t>
   </si>
   <si>
@@ -1214,13 +1196,316 @@
     <t>Dormir / Se réveiller</t>
   </si>
   <si>
-    <t>Choisir une direction</t>
-  </si>
-  <si>
     <t>Machine (Organisme)</t>
   </si>
   <si>
     <t>Machine (Environnement)</t>
+  </si>
+  <si>
+    <t>Changer la température</t>
+  </si>
+  <si>
+    <t>Modifier sa température</t>
+  </si>
+  <si>
+    <t>Corps régule sa température ou cesse de réguler</t>
+  </si>
+  <si>
+    <t>Changer le taux d'humidité</t>
+  </si>
+  <si>
+    <t>Modifier le taux d'humidité</t>
+  </si>
+  <si>
+    <t>Corps se met en cryptobiose au besoin</t>
+  </si>
+  <si>
+    <t>Ajustement de l'état de transitions</t>
+  </si>
+  <si>
+    <t>Enregistrement épigénétique au besoin</t>
+  </si>
+  <si>
+    <t>Appliquer les nuages</t>
+  </si>
+  <si>
+    <t>Ajouter un autre type de nuage</t>
+  </si>
+  <si>
+    <t>Machine (Interface)</t>
+  </si>
+  <si>
+    <t>Ajouter une plage de nuage</t>
+  </si>
+  <si>
+    <t>Créer les nuages aléatoirement dans le modèle</t>
+  </si>
+  <si>
+    <t>Faire bouger les nuages</t>
+  </si>
+  <si>
+    <t>Déterminer vitesse et direction du vent (changeant)</t>
+  </si>
+  <si>
+    <t>Choisir les paramètre du nuage (intensité du centre, rayon total, rayon du centre, nombre)</t>
+  </si>
+  <si>
+    <t>Mécanorécepteurs envoient un signal au système nerveux</t>
+  </si>
+  <si>
+    <t>Thermorécepteurs envoient un signal au système nerveux (en continu)</t>
+  </si>
+  <si>
+    <t>Système nerveux vérifie la température du corps et lui envoie un signal au besoin (en continu)</t>
+  </si>
+  <si>
+    <t>Hygrorécepteur envoie un signal au système nerveux (en continu)</t>
+  </si>
+  <si>
+    <t>Système nerveux vérifie capacité de l'organisme à tolérer ce taux d'humidité (en continu)</t>
+  </si>
+  <si>
+    <t>Détecte un changement de température</t>
+  </si>
+  <si>
+    <t>Détecte un changement du taux d'humidité</t>
+  </si>
+  <si>
+    <t>Détecte un nuage au-dessus de lui</t>
+  </si>
+  <si>
+    <t>Système nerveux vérifie quels mécanorécepteurs reçoient le plus de signaux</t>
+  </si>
+  <si>
+    <t>Ajuste l'orientation</t>
+  </si>
+  <si>
+    <t>Boucle de vérification (deux étapes précédentes)</t>
+  </si>
+  <si>
+    <t>Avance pour fuir le nuage</t>
+  </si>
+  <si>
+    <t>Changer ou enlever des nuages</t>
+  </si>
+  <si>
+    <t>Ajuste la quantité de nuage et leurs paramètres dans le modèle</t>
+  </si>
+  <si>
+    <t>Ajuster la plage de nuage</t>
+  </si>
+  <si>
+    <t>Faire apparaître de la nourriture aléatoirement</t>
+  </si>
+  <si>
+    <t>Supprimer de la nourriture aléatoirement</t>
+  </si>
+  <si>
+    <t>Changement de ratio terre / eau</t>
+  </si>
+  <si>
+    <t>Quantité de nourriture / vitesse d'apparition</t>
+  </si>
+  <si>
+    <t>Changer la quantité de nourriture</t>
+  </si>
+  <si>
+    <t>Chronomètre pour la vitesse d'apparition de nourriture</t>
+  </si>
+  <si>
+    <t>Odorat détecte de la nourriture et envoie un signal au système nerveux</t>
+  </si>
+  <si>
+    <t>Système nerveux change l'orientation de l'organisme pour tenter de voir la nourriture</t>
+  </si>
+  <si>
+    <t>Si la nourriture est dans le champ de vision, la organisme se déplace</t>
+  </si>
+  <si>
+    <t>Si la nourriture est dans la portée de la organisme, la organisme mange</t>
+  </si>
+  <si>
+    <t>Changer le ratio</t>
+  </si>
+  <si>
+    <t>Ajustement aléatoire dans le modèle</t>
+  </si>
+  <si>
+    <t>Détection de la faim de l'organisme (jauge de faim)</t>
+  </si>
+  <si>
+    <t>Détection de la soif de l'organisme (jauge de soif)</t>
+  </si>
+  <si>
+    <t>** La suite : même chose que pour manger</t>
+  </si>
+  <si>
+    <t>Ajustement du système digestif</t>
+  </si>
+  <si>
+    <t>Déféquer / uriner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Système digestif détecte si liquide ou solide </t>
+  </si>
+  <si>
+    <t>Ajustement des jauges faim / soif</t>
+  </si>
+  <si>
+    <t>Stockage dans le bon organe</t>
+  </si>
+  <si>
+    <t>Évacuation au bout d'un certain temps ou lorsque le stockage est plein</t>
+  </si>
+  <si>
+    <t>Absorption des aliments</t>
+  </si>
+  <si>
+    <t>Choisir tous les paramètres ci-haut</t>
+  </si>
+  <si>
+    <t>Choisir la durée</t>
+  </si>
+  <si>
+    <t>Ajustement de l'interface</t>
+  </si>
+  <si>
+    <t>Appliquer les changements</t>
+  </si>
+  <si>
+    <t>Automatiser les changements de paramètres (chrono + boucle)</t>
+  </si>
+  <si>
+    <t>Création d'un cycle (saisons)</t>
+  </si>
+  <si>
+    <t>Appliquer le cycle</t>
+  </si>
+  <si>
+    <t>Déplacement des nuages</t>
+  </si>
+  <si>
+    <t>Génération de la nourriture</t>
+  </si>
+  <si>
+    <t>Détecter fin de cycle</t>
+  </si>
+  <si>
+    <t>Changer les paramètres de l'environnement (graduellement)</t>
+  </si>
+  <si>
+    <t>Détectection des besoins</t>
+  </si>
+  <si>
+    <t>Vérification de la priorité des besoins</t>
+  </si>
+  <si>
+    <t>Système nerveux active d'une action pour répondre au besoin prioritaire</t>
+  </si>
+  <si>
+    <t>Fluctuation des jauges de besoin selon le temps, l'environnement, les événements, l'organisme</t>
+  </si>
+  <si>
+    <t>Vieillir</t>
+  </si>
+  <si>
+    <t>Naître</t>
+  </si>
+  <si>
+    <t>Apparaître (et déterminer la génétique)</t>
+  </si>
+  <si>
+    <t>Activation de la jauge santé</t>
+  </si>
+  <si>
+    <t>Déterminer le seuil de vieillissement</t>
+  </si>
+  <si>
+    <t>Réduction de la jauge santé dépassé un certain seuil (méthode = parabole)</t>
+  </si>
+  <si>
+    <t>Vérication de la jauge de santé</t>
+  </si>
+  <si>
+    <t>Meurt si jauge santé = 0</t>
+  </si>
+  <si>
+    <t>Supprimer l'organisme du modèle</t>
+  </si>
+  <si>
+    <t>Chercher à se reproduire</t>
+  </si>
+  <si>
+    <t>Si la recherche est active : émission de phéromones</t>
+  </si>
+  <si>
+    <t>Si odorat détecte phéromones, même chose que pour la faim</t>
+  </si>
+  <si>
+    <t>Début de gestation : assemblage des gènes</t>
+  </si>
+  <si>
+    <t>Deux organismes se reproduisent</t>
+  </si>
+  <si>
+    <t>Vérification de l'épigénétique et de l'intensité du trauma intergénérationnel</t>
+  </si>
+  <si>
+    <t>Vérification de la transformation de l'épigénétique en génétique innée</t>
+  </si>
+  <si>
+    <t>Faire apparaître un organisme</t>
+  </si>
+  <si>
+    <t>Détermination finale de la génétique et des attributs de l'organisme</t>
+  </si>
+  <si>
+    <t>Se mettre en état de sommeil en cas de besoin</t>
+  </si>
+  <si>
+    <t>Ajustement de la jauge de faim et d'énergie de l'organisme</t>
+  </si>
+  <si>
+    <t>Détection de la jauge d'énergie</t>
+  </si>
+  <si>
+    <t>Augmentation de la jauge d'énergie</t>
+  </si>
+  <si>
+    <t>Ajustement de la jauge énergie en conséquence</t>
+  </si>
+  <si>
+    <t>Choisir une orientation</t>
+  </si>
+  <si>
+    <t>Changer la taille du monde</t>
+  </si>
+  <si>
+    <t>Faire défiler l'écran</t>
+  </si>
+  <si>
+    <t>Bouger ce qui est vu dans le modèle</t>
+  </si>
+  <si>
+    <t>Agrandir ou réduire la taille de la fenêtre</t>
+  </si>
+  <si>
+    <t>Ajuster la vue</t>
+  </si>
+  <si>
+    <t>Ajuster les proportions de la vue</t>
+  </si>
+  <si>
+    <t>Afficher informations d'un organisme</t>
+  </si>
+  <si>
+    <t>Cliquer sur un organisme</t>
+  </si>
+  <si>
+    <t>Aller chercher les infos de l'organisme</t>
+  </si>
+  <si>
+    <t>Afficher les infos de l'organisme</t>
   </si>
 </sst>
 </file>
@@ -1403,7 +1688,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="72">
+  <borders count="70">
     <border>
       <left/>
       <right/>
@@ -2188,41 +2473,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="234">
+  <cellXfs count="228">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2592,55 +2847,6 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2653,19 +2859,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2713,33 +2907,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="71" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2770,15 +2945,75 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3475,22 +3710,22 @@
       </c>
     </row>
     <row r="36" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F36" s="165"/>
-      <c r="G36" s="166"/>
-      <c r="H36" s="166"/>
-      <c r="I36" s="166"/>
+      <c r="F36" s="205"/>
+      <c r="G36" s="206"/>
+      <c r="H36" s="206"/>
+      <c r="I36" s="206"/>
     </row>
     <row r="37" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F37" s="166"/>
-      <c r="G37" s="166"/>
-      <c r="H37" s="166"/>
-      <c r="I37" s="166"/>
+      <c r="F37" s="206"/>
+      <c r="G37" s="206"/>
+      <c r="H37" s="206"/>
+      <c r="I37" s="206"/>
     </row>
     <row r="38" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F38" s="166"/>
-      <c r="G38" s="166"/>
-      <c r="H38" s="166"/>
-      <c r="I38" s="166"/>
+      <c r="F38" s="206"/>
+      <c r="G38" s="206"/>
+      <c r="H38" s="206"/>
+      <c r="I38" s="206"/>
     </row>
     <row r="39" spans="6:9" ht="17.25" customHeight="1">
       <c r="F39" s="82"/>
@@ -3499,22 +3734,22 @@
       <c r="I39" s="82"/>
     </row>
     <row r="40" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F40" s="165"/>
-      <c r="G40" s="166"/>
-      <c r="H40" s="166"/>
-      <c r="I40" s="166"/>
+      <c r="F40" s="205"/>
+      <c r="G40" s="206"/>
+      <c r="H40" s="206"/>
+      <c r="I40" s="206"/>
     </row>
     <row r="41" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F41" s="166"/>
-      <c r="G41" s="166"/>
-      <c r="H41" s="166"/>
-      <c r="I41" s="166"/>
+      <c r="F41" s="206"/>
+      <c r="G41" s="206"/>
+      <c r="H41" s="206"/>
+      <c r="I41" s="206"/>
     </row>
     <row r="42" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F42" s="166"/>
-      <c r="G42" s="166"/>
-      <c r="H42" s="166"/>
-      <c r="I42" s="166"/>
+      <c r="F42" s="206"/>
+      <c r="G42" s="206"/>
+      <c r="H42" s="206"/>
+      <c r="I42" s="206"/>
     </row>
     <row r="43" spans="6:9" ht="17.25" customHeight="1">
       <c r="F43" s="82"/>
@@ -3529,34 +3764,34 @@
       <c r="I44" s="82"/>
     </row>
     <row r="45" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F45" s="165"/>
-      <c r="G45" s="166"/>
-      <c r="H45" s="166"/>
-      <c r="I45" s="166"/>
+      <c r="F45" s="205"/>
+      <c r="G45" s="206"/>
+      <c r="H45" s="206"/>
+      <c r="I45" s="206"/>
     </row>
     <row r="46" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F46" s="166"/>
-      <c r="G46" s="166"/>
-      <c r="H46" s="166"/>
-      <c r="I46" s="166"/>
+      <c r="F46" s="206"/>
+      <c r="G46" s="206"/>
+      <c r="H46" s="206"/>
+      <c r="I46" s="206"/>
     </row>
     <row r="47" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F47" s="166"/>
-      <c r="G47" s="166"/>
-      <c r="H47" s="166"/>
-      <c r="I47" s="166"/>
+      <c r="F47" s="206"/>
+      <c r="G47" s="206"/>
+      <c r="H47" s="206"/>
+      <c r="I47" s="206"/>
     </row>
     <row r="48" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F48" s="166"/>
-      <c r="G48" s="166"/>
-      <c r="H48" s="166"/>
-      <c r="I48" s="166"/>
+      <c r="F48" s="206"/>
+      <c r="G48" s="206"/>
+      <c r="H48" s="206"/>
+      <c r="I48" s="206"/>
     </row>
     <row r="49" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F49" s="166"/>
-      <c r="G49" s="166"/>
-      <c r="H49" s="166"/>
-      <c r="I49" s="166"/>
+      <c r="F49" s="206"/>
+      <c r="G49" s="206"/>
+      <c r="H49" s="206"/>
+      <c r="I49" s="206"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3679,7 +3914,7 @@
       </c>
     </row>
     <row r="13" spans="2:8" ht="12.75" customHeight="1">
-      <c r="B13" s="167" t="s">
+      <c r="B13" s="207" t="s">
         <v>60</v>
       </c>
       <c r="C13" s="142"/>
@@ -3688,7 +3923,7 @@
       <c r="H13" s="163"/>
     </row>
     <row r="14" spans="2:8" ht="12.75" customHeight="1">
-      <c r="B14" s="168"/>
+      <c r="B14" s="208"/>
       <c r="C14" s="143" t="s">
         <v>158</v>
       </c>
@@ -3701,13 +3936,13 @@
       <c r="H14" s="163"/>
     </row>
     <row r="15" spans="2:8" ht="12.75" customHeight="1">
-      <c r="B15" s="168"/>
+      <c r="B15" s="208"/>
       <c r="C15" s="146"/>
       <c r="D15" s="144"/>
       <c r="E15" s="145"/>
     </row>
     <row r="16" spans="2:8" ht="12.75" customHeight="1">
-      <c r="B16" s="168"/>
+      <c r="B16" s="208"/>
       <c r="C16" s="156" t="s">
         <v>225</v>
       </c>
@@ -3719,7 +3954,7 @@
       </c>
     </row>
     <row r="17" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B17" s="169"/>
+      <c r="B17" s="209"/>
       <c r="C17" s="146" t="s">
         <v>155</v>
       </c>
@@ -3727,7 +3962,7 @@
       <c r="E17" s="145"/>
     </row>
     <row r="18" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B18" s="169"/>
+      <c r="B18" s="209"/>
       <c r="C18" s="156" t="s">
         <v>226</v>
       </c>
@@ -3737,13 +3972,13 @@
       </c>
     </row>
     <row r="19" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B19" s="169"/>
+      <c r="B19" s="209"/>
       <c r="C19" s="146"/>
       <c r="D19" s="144"/>
       <c r="E19" s="145"/>
     </row>
     <row r="20" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B20" s="169"/>
+      <c r="B20" s="209"/>
       <c r="C20" s="143" t="s">
         <v>159</v>
       </c>
@@ -3755,13 +3990,13 @@
       </c>
     </row>
     <row r="21" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B21" s="169"/>
+      <c r="B21" s="209"/>
       <c r="C21" s="146"/>
       <c r="D21" s="144"/>
       <c r="E21" s="145"/>
     </row>
     <row r="22" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B22" s="169"/>
+      <c r="B22" s="209"/>
       <c r="C22" s="156" t="s">
         <v>228</v>
       </c>
@@ -3773,7 +4008,7 @@
       </c>
     </row>
     <row r="23" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B23" s="169"/>
+      <c r="B23" s="209"/>
       <c r="C23" s="161" t="s">
         <v>164</v>
       </c>
@@ -3785,7 +4020,7 @@
       </c>
     </row>
     <row r="24" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B24" s="169"/>
+      <c r="B24" s="209"/>
       <c r="C24" s="146"/>
       <c r="D24" s="157" t="s">
         <v>230</v>
@@ -3793,7 +4028,7 @@
       <c r="E24" s="158"/>
     </row>
     <row r="25" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B25" s="169"/>
+      <c r="B25" s="209"/>
       <c r="C25" s="156"/>
       <c r="D25" s="157" t="s">
         <v>167</v>
@@ -3801,7 +4036,7 @@
       <c r="E25" s="158"/>
     </row>
     <row r="26" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B26" s="169"/>
+      <c r="B26" s="209"/>
       <c r="C26" s="156" t="s">
         <v>168</v>
       </c>
@@ -3811,7 +4046,7 @@
       </c>
     </row>
     <row r="27" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B27" s="169"/>
+      <c r="B27" s="209"/>
       <c r="C27" s="156" t="s">
         <v>170</v>
       </c>
@@ -3821,13 +4056,13 @@
       </c>
     </row>
     <row r="28" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B28" s="169"/>
+      <c r="B28" s="209"/>
       <c r="C28" s="146"/>
       <c r="D28" s="144"/>
       <c r="E28" s="145"/>
     </row>
     <row r="29" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B29" s="169"/>
+      <c r="B29" s="209"/>
       <c r="C29" s="143" t="s">
         <v>172</v>
       </c>
@@ -3835,13 +4070,13 @@
       <c r="E29" s="145"/>
     </row>
     <row r="30" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B30" s="169"/>
+      <c r="B30" s="209"/>
       <c r="C30" s="146"/>
       <c r="D30" s="144"/>
       <c r="E30" s="145"/>
     </row>
     <row r="31" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B31" s="169"/>
+      <c r="B31" s="209"/>
       <c r="C31" s="156" t="s">
         <v>173</v>
       </c>
@@ -3851,7 +4086,7 @@
       <c r="E31" s="145"/>
     </row>
     <row r="32" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B32" s="169"/>
+      <c r="B32" s="209"/>
       <c r="C32" s="156" t="s">
         <v>174</v>
       </c>
@@ -3859,7 +4094,7 @@
       <c r="E32" s="145"/>
     </row>
     <row r="33" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B33" s="169"/>
+      <c r="B33" s="209"/>
       <c r="C33" s="156" t="s">
         <v>175</v>
       </c>
@@ -3867,7 +4102,7 @@
       <c r="E33" s="145"/>
     </row>
     <row r="34" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B34" s="169"/>
+      <c r="B34" s="209"/>
       <c r="C34" s="156" t="s">
         <v>176</v>
       </c>
@@ -3875,7 +4110,7 @@
       <c r="E34" s="145"/>
     </row>
     <row r="35" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B35" s="169"/>
+      <c r="B35" s="209"/>
       <c r="C35" s="156" t="s">
         <v>177</v>
       </c>
@@ -3883,13 +4118,13 @@
       <c r="E35" s="145"/>
     </row>
     <row r="36" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B36" s="169"/>
+      <c r="B36" s="209"/>
       <c r="C36" s="156"/>
       <c r="D36" s="157"/>
       <c r="E36" s="145"/>
     </row>
     <row r="37" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B37" s="169"/>
+      <c r="B37" s="209"/>
       <c r="C37" s="156" t="s">
         <v>231</v>
       </c>
@@ -3897,7 +4132,7 @@
       <c r="E37" s="145"/>
     </row>
     <row r="38" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B38" s="169"/>
+      <c r="B38" s="209"/>
       <c r="C38" s="156" t="s">
         <v>181</v>
       </c>
@@ -3905,7 +4140,7 @@
       <c r="E38" s="145"/>
     </row>
     <row r="39" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B39" s="169"/>
+      <c r="B39" s="209"/>
       <c r="C39" s="156" t="s">
         <v>179</v>
       </c>
@@ -3915,13 +4150,13 @@
       </c>
     </row>
     <row r="40" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B40" s="169"/>
+      <c r="B40" s="209"/>
       <c r="C40" s="156"/>
       <c r="D40" s="144"/>
       <c r="E40" s="145"/>
     </row>
     <row r="41" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B41" s="169"/>
+      <c r="B41" s="209"/>
       <c r="C41" s="143" t="s">
         <v>182</v>
       </c>
@@ -3929,13 +4164,13 @@
       <c r="E41" s="145"/>
     </row>
     <row r="42" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B42" s="169"/>
+      <c r="B42" s="209"/>
       <c r="C42" s="156"/>
       <c r="D42" s="144"/>
       <c r="E42" s="145"/>
     </row>
     <row r="43" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B43" s="169"/>
+      <c r="B43" s="209"/>
       <c r="C43" s="156" t="s">
         <v>183</v>
       </c>
@@ -3943,7 +4178,7 @@
       <c r="E43" s="145"/>
     </row>
     <row r="44" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B44" s="169"/>
+      <c r="B44" s="209"/>
       <c r="C44" s="156" t="s">
         <v>155</v>
       </c>
@@ -3953,7 +4188,7 @@
       <c r="E44" s="145"/>
     </row>
     <row r="45" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B45" s="169"/>
+      <c r="B45" s="209"/>
       <c r="C45" s="156" t="s">
         <v>185</v>
       </c>
@@ -3963,7 +4198,7 @@
       <c r="E45" s="145"/>
     </row>
     <row r="46" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B46" s="169"/>
+      <c r="B46" s="209"/>
       <c r="C46" s="156" t="s">
         <v>187</v>
       </c>
@@ -3973,7 +4208,7 @@
       <c r="E46" s="145"/>
     </row>
     <row r="47" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B47" s="169"/>
+      <c r="B47" s="209"/>
       <c r="C47" s="156" t="s">
         <v>189</v>
       </c>
@@ -3983,7 +4218,7 @@
       </c>
     </row>
     <row r="48" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B48" s="169"/>
+      <c r="B48" s="209"/>
       <c r="C48" s="161" t="s">
         <v>191</v>
       </c>
@@ -3991,7 +4226,7 @@
       <c r="E48" s="145"/>
     </row>
     <row r="49" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B49" s="169"/>
+      <c r="B49" s="209"/>
       <c r="C49" s="161" t="s">
         <v>192</v>
       </c>
@@ -3999,13 +4234,13 @@
       <c r="E49" s="145"/>
     </row>
     <row r="50" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B50" s="169"/>
+      <c r="B50" s="209"/>
       <c r="C50" s="156"/>
       <c r="D50" s="144"/>
       <c r="E50" s="145"/>
     </row>
     <row r="51" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B51" s="169"/>
+      <c r="B51" s="209"/>
       <c r="C51" s="143" t="s">
         <v>193</v>
       </c>
@@ -4013,13 +4248,13 @@
       <c r="E51" s="145"/>
     </row>
     <row r="52" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B52" s="169"/>
+      <c r="B52" s="209"/>
       <c r="C52" s="156"/>
       <c r="D52" s="144"/>
       <c r="E52" s="145"/>
     </row>
     <row r="53" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B53" s="169"/>
+      <c r="B53" s="209"/>
       <c r="C53" s="156" t="s">
         <v>194</v>
       </c>
@@ -4029,7 +4264,7 @@
       </c>
     </row>
     <row r="54" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B54" s="169"/>
+      <c r="B54" s="209"/>
       <c r="C54" s="156" t="s">
         <v>196</v>
       </c>
@@ -4037,7 +4272,7 @@
       <c r="E54" s="145"/>
     </row>
     <row r="55" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B55" s="169"/>
+      <c r="B55" s="209"/>
       <c r="C55" s="156" t="s">
         <v>197</v>
       </c>
@@ -4045,7 +4280,7 @@
       <c r="E55" s="145"/>
     </row>
     <row r="56" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B56" s="169"/>
+      <c r="B56" s="209"/>
       <c r="C56" s="156" t="s">
         <v>198</v>
       </c>
@@ -4053,7 +4288,7 @@
       <c r="E56" s="145"/>
     </row>
     <row r="57" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B57" s="169"/>
+      <c r="B57" s="209"/>
       <c r="C57" s="156" t="s">
         <v>199</v>
       </c>
@@ -4061,7 +4296,7 @@
       <c r="E57" s="145"/>
     </row>
     <row r="58" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B58" s="169"/>
+      <c r="B58" s="209"/>
       <c r="C58" s="156" t="s">
         <v>200</v>
       </c>
@@ -4071,7 +4306,7 @@
       <c r="E58" s="145"/>
     </row>
     <row r="59" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B59" s="169"/>
+      <c r="B59" s="209"/>
       <c r="C59" s="156" t="s">
         <v>192</v>
       </c>
@@ -4081,7 +4316,7 @@
       <c r="E59" s="145"/>
     </row>
     <row r="60" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B60" s="169"/>
+      <c r="B60" s="209"/>
       <c r="C60" s="156" t="s">
         <v>203</v>
       </c>
@@ -4089,7 +4324,7 @@
       <c r="E60" s="145"/>
     </row>
     <row r="61" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B61" s="169"/>
+      <c r="B61" s="209"/>
       <c r="C61" s="156" t="s">
         <v>204</v>
       </c>
@@ -4099,7 +4334,7 @@
       </c>
     </row>
     <row r="62" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B62" s="169"/>
+      <c r="B62" s="209"/>
       <c r="C62" s="156" t="s">
         <v>206</v>
       </c>
@@ -4107,13 +4342,13 @@
       <c r="E62" s="145"/>
     </row>
     <row r="63" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B63" s="169"/>
+      <c r="B63" s="209"/>
       <c r="C63" s="156"/>
       <c r="D63" s="144"/>
       <c r="E63" s="145"/>
     </row>
     <row r="64" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B64" s="169"/>
+      <c r="B64" s="209"/>
       <c r="C64" s="143" t="s">
         <v>207</v>
       </c>
@@ -4121,13 +4356,13 @@
       <c r="E64" s="145"/>
     </row>
     <row r="65" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B65" s="169"/>
+      <c r="B65" s="209"/>
       <c r="C65" s="156"/>
       <c r="D65" s="144"/>
       <c r="E65" s="145"/>
     </row>
     <row r="66" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B66" s="169"/>
+      <c r="B66" s="209"/>
       <c r="C66" s="156" t="s">
         <v>209</v>
       </c>
@@ -4135,7 +4370,7 @@
       <c r="E66" s="145"/>
     </row>
     <row r="67" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B67" s="169"/>
+      <c r="B67" s="209"/>
       <c r="C67" s="156" t="s">
         <v>210</v>
       </c>
@@ -4143,7 +4378,7 @@
       <c r="E67" s="145"/>
     </row>
     <row r="68" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B68" s="169"/>
+      <c r="B68" s="209"/>
       <c r="C68" s="156" t="s">
         <v>208</v>
       </c>
@@ -4151,7 +4386,7 @@
       <c r="E68" s="145"/>
     </row>
     <row r="69" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B69" s="169"/>
+      <c r="B69" s="209"/>
       <c r="C69" s="156" t="s">
         <v>211</v>
       </c>
@@ -4159,25 +4394,25 @@
       <c r="E69" s="145"/>
     </row>
     <row r="70" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B70" s="169"/>
+      <c r="B70" s="209"/>
       <c r="C70" s="156"/>
       <c r="D70" s="144"/>
       <c r="E70" s="145"/>
     </row>
     <row r="71" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B71" s="169"/>
+      <c r="B71" s="209"/>
       <c r="C71" s="156"/>
       <c r="D71" s="144"/>
       <c r="E71" s="145"/>
     </row>
     <row r="72" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B72" s="170"/>
+      <c r="B72" s="210"/>
       <c r="C72" s="147"/>
       <c r="D72" s="148"/>
       <c r="E72" s="149"/>
     </row>
     <row r="73" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B73" s="167" t="s">
+      <c r="B73" s="207" t="s">
         <v>61</v>
       </c>
       <c r="C73" s="156"/>
@@ -4189,7 +4424,7 @@
       </c>
     </row>
     <row r="74" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B74" s="169"/>
+      <c r="B74" s="209"/>
       <c r="C74" s="156" t="s">
         <v>242</v>
       </c>
@@ -4201,7 +4436,7 @@
       </c>
     </row>
     <row r="75" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B75" s="169"/>
+      <c r="B75" s="209"/>
       <c r="C75" s="146"/>
       <c r="D75" s="157" t="s">
         <v>216</v>
@@ -4211,7 +4446,7 @@
       </c>
     </row>
     <row r="76" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B76" s="169"/>
+      <c r="B76" s="209"/>
       <c r="C76" s="146"/>
       <c r="D76" s="144" t="s">
         <v>156</v>
@@ -4221,7 +4456,7 @@
       </c>
     </row>
     <row r="77" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B77" s="169"/>
+      <c r="B77" s="209"/>
       <c r="C77" s="146"/>
       <c r="D77" s="144" t="s">
         <v>157</v>
@@ -4231,7 +4466,7 @@
       </c>
     </row>
     <row r="78" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B78" s="169"/>
+      <c r="B78" s="209"/>
       <c r="C78" s="146"/>
       <c r="D78" s="157" t="s">
         <v>160</v>
@@ -4241,7 +4476,7 @@
       </c>
     </row>
     <row r="79" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B79" s="169"/>
+      <c r="B79" s="209"/>
       <c r="C79" s="146"/>
       <c r="D79" s="157" t="s">
         <v>233</v>
@@ -4251,7 +4486,7 @@
       </c>
     </row>
     <row r="80" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B80" s="169"/>
+      <c r="B80" s="209"/>
       <c r="C80" s="146"/>
       <c r="D80" s="157" t="s">
         <v>212</v>
@@ -4261,7 +4496,7 @@
       </c>
     </row>
     <row r="81" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B81" s="169"/>
+      <c r="B81" s="209"/>
       <c r="C81" s="146"/>
       <c r="D81" s="157" t="s">
         <v>213</v>
@@ -4271,7 +4506,7 @@
       </c>
     </row>
     <row r="82" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B82" s="169"/>
+      <c r="B82" s="209"/>
       <c r="C82" s="146"/>
       <c r="D82" s="157" t="s">
         <v>214</v>
@@ -4281,7 +4516,7 @@
       </c>
     </row>
     <row r="83" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B83" s="169"/>
+      <c r="B83" s="209"/>
       <c r="C83" s="156"/>
       <c r="D83" s="157" t="s">
         <v>234</v>
@@ -4291,7 +4526,7 @@
       </c>
     </row>
     <row r="84" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B84" s="169"/>
+      <c r="B84" s="209"/>
       <c r="C84" s="156"/>
       <c r="D84" s="157" t="s">
         <v>235</v>
@@ -4301,7 +4536,7 @@
       </c>
     </row>
     <row r="85" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B85" s="169"/>
+      <c r="B85" s="209"/>
       <c r="C85" s="146"/>
       <c r="D85" s="157" t="s">
         <v>236</v>
@@ -4311,7 +4546,7 @@
       </c>
     </row>
     <row r="86" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B86" s="169"/>
+      <c r="B86" s="209"/>
       <c r="C86" s="146"/>
       <c r="D86" s="157" t="s">
         <v>238</v>
@@ -4321,7 +4556,7 @@
       </c>
     </row>
     <row r="87" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B87" s="169"/>
+      <c r="B87" s="209"/>
       <c r="C87" s="146"/>
       <c r="D87" s="157" t="s">
         <v>247</v>
@@ -4331,7 +4566,7 @@
       </c>
     </row>
     <row r="88" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B88" s="169"/>
+      <c r="B88" s="209"/>
       <c r="C88" s="146"/>
       <c r="D88" s="157" t="s">
         <v>248</v>
@@ -4341,13 +4576,13 @@
       </c>
     </row>
     <row r="89" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B89" s="170"/>
+      <c r="B89" s="210"/>
       <c r="C89" s="147"/>
       <c r="D89" s="148"/>
       <c r="E89" s="149"/>
     </row>
     <row r="90" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B90" s="167" t="s">
+      <c r="B90" s="207" t="s">
         <v>62</v>
       </c>
       <c r="C90" s="150"/>
@@ -4355,7 +4590,7 @@
       <c r="E90" s="152"/>
     </row>
     <row r="91" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B91" s="169"/>
+      <c r="B91" s="209"/>
       <c r="C91" s="156" t="s">
         <v>243</v>
       </c>
@@ -4363,7 +4598,7 @@
       <c r="E91" s="145"/>
     </row>
     <row r="92" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B92" s="169"/>
+      <c r="B92" s="209"/>
       <c r="C92" s="156" t="s">
         <v>244</v>
       </c>
@@ -4371,7 +4606,7 @@
       <c r="E92" s="145"/>
     </row>
     <row r="93" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B93" s="169"/>
+      <c r="B93" s="209"/>
       <c r="C93" s="146" t="s">
         <v>245</v>
       </c>
@@ -4379,37 +4614,37 @@
       <c r="E93" s="145"/>
     </row>
     <row r="94" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B94" s="169"/>
+      <c r="B94" s="209"/>
       <c r="C94" s="146"/>
       <c r="D94" s="144"/>
       <c r="E94" s="145"/>
     </row>
     <row r="95" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B95" s="169"/>
+      <c r="B95" s="209"/>
       <c r="C95" s="146"/>
       <c r="D95" s="144"/>
       <c r="E95" s="145"/>
     </row>
     <row r="96" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B96" s="169"/>
+      <c r="B96" s="209"/>
       <c r="C96" s="146"/>
       <c r="D96" s="144"/>
       <c r="E96" s="145"/>
     </row>
     <row r="97" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B97" s="169"/>
+      <c r="B97" s="209"/>
       <c r="C97" s="146"/>
       <c r="D97" s="144"/>
       <c r="E97" s="145"/>
     </row>
     <row r="98" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B98" s="169"/>
+      <c r="B98" s="209"/>
       <c r="C98" s="146"/>
       <c r="D98" s="144"/>
       <c r="E98" s="145"/>
     </row>
     <row r="99" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B99" s="170"/>
+      <c r="B99" s="210"/>
       <c r="C99" s="153"/>
       <c r="D99" s="154"/>
       <c r="E99" s="155"/>
@@ -4463,26 +4698,26 @@
     </row>
     <row r="3" spans="2:9" ht="56.25" customHeight="1">
       <c r="B3" s="80"/>
-      <c r="C3" s="171" t="s">
+      <c r="C3" s="211" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="171"/>
-      <c r="E3" s="171"/>
-      <c r="F3" s="171"/>
-      <c r="G3" s="171"/>
-      <c r="H3" s="171"/>
-      <c r="I3" s="171"/>
+      <c r="D3" s="211"/>
+      <c r="E3" s="211"/>
+      <c r="F3" s="211"/>
+      <c r="G3" s="211"/>
+      <c r="H3" s="211"/>
+      <c r="I3" s="211"/>
     </row>
     <row r="4" spans="2:9" ht="30.75" customHeight="1">
       <c r="B4" s="81"/>
-      <c r="C4" s="172" t="s">
+      <c r="C4" s="212" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="172"/>
-      <c r="E4" s="172"/>
-      <c r="F4" s="172"/>
-      <c r="G4" s="166"/>
-      <c r="H4" s="166"/>
+      <c r="D4" s="212"/>
+      <c r="E4" s="212"/>
+      <c r="F4" s="212"/>
+      <c r="G4" s="206"/>
+      <c r="H4" s="206"/>
       <c r="I4" s="81"/>
     </row>
     <row r="5" spans="2:9" ht="21" customHeight="1">
@@ -4681,79 +4916,80 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:G88"/>
+  <dimension ref="B1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D122" sqref="D122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="225" customWidth="1"/>
-    <col min="3" max="3" width="49.28515625" customWidth="1"/>
-    <col min="4" max="4" width="44.42578125" customWidth="1"/>
-    <col min="5" max="6" width="49.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="197" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" customWidth="1"/>
+    <col min="4" max="4" width="108.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.7109375" customWidth="1"/>
+    <col min="6" max="6" width="72" customWidth="1"/>
     <col min="7" max="7" width="49.28515625" customWidth="1"/>
     <col min="8" max="9" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:7" ht="20.25" customHeight="1" thickBot="1">
-      <c r="B2" s="226"/>
-      <c r="C2" s="182" t="s">
+      <c r="B2" s="198"/>
+      <c r="C2" s="165" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="183"/>
-      <c r="E2" s="184"/>
-      <c r="F2" s="184"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
       <c r="G2" s="80"/>
     </row>
-    <row r="3" spans="2:7" s="189" customFormat="1" ht="56.25" customHeight="1">
-      <c r="B3" s="227"/>
-      <c r="C3" s="186" t="s">
+    <row r="3" spans="2:7" s="169" customFormat="1" ht="56.25" customHeight="1">
+      <c r="B3" s="199"/>
+      <c r="C3" s="213" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="187"/>
-      <c r="E3" s="188"/>
-      <c r="G3" s="185"/>
-    </row>
-    <row r="4" spans="2:7" s="189" customFormat="1" ht="30.75" customHeight="1">
-      <c r="B4" s="227"/>
-      <c r="C4" s="190" t="s">
+      <c r="D3" s="214"/>
+      <c r="E3" s="215"/>
+      <c r="G3" s="168"/>
+    </row>
+    <row r="4" spans="2:7" s="169" customFormat="1" ht="30.75" customHeight="1">
+      <c r="B4" s="199"/>
+      <c r="C4" s="216" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="187"/>
-      <c r="E4" s="188"/>
+      <c r="D4" s="214"/>
+      <c r="E4" s="215"/>
     </row>
     <row r="5" spans="2:7" ht="21" customHeight="1">
-      <c r="B5" s="226"/>
-      <c r="C5" s="191" t="s">
+      <c r="B5" s="198"/>
+      <c r="C5" s="170" t="s">
         <v>66</v>
       </c>
       <c r="D5" s="80"/>
-      <c r="E5" s="192"/>
-      <c r="F5" s="192"/>
+      <c r="E5" s="171"/>
+      <c r="F5" s="171"/>
     </row>
     <row r="6" spans="2:7" ht="21" customHeight="1" thickBot="1">
-      <c r="B6" s="228"/>
-      <c r="C6" s="193" t="s">
+      <c r="B6" s="200"/>
+      <c r="C6" s="172" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="194"/>
-      <c r="E6" s="195"/>
-      <c r="F6" s="195"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="174"/>
+      <c r="F6" s="174"/>
     </row>
     <row r="7" spans="2:7" ht="18" customHeight="1">
-      <c r="B7" s="228"/>
+      <c r="B7" s="200"/>
       <c r="C7" s="82"/>
       <c r="D7" s="82"/>
       <c r="E7" s="82"/>
       <c r="F7" s="82"/>
     </row>
     <row r="8" spans="2:7" ht="18" customHeight="1">
-      <c r="B8" s="228"/>
-      <c r="C8" s="196" t="s">
+      <c r="B8" s="200"/>
+      <c r="C8" s="175" t="s">
         <v>249</v>
       </c>
       <c r="D8" s="27"/>
@@ -4761,20 +4997,20 @@
       <c r="F8" s="82"/>
     </row>
     <row r="9" spans="2:7" ht="19.5" customHeight="1">
-      <c r="B9" s="228"/>
-      <c r="C9" s="197" t="s">
+      <c r="B9" s="200"/>
+      <c r="C9" s="176" t="s">
         <v>250</v>
       </c>
-      <c r="D9" s="198"/>
+      <c r="D9" s="177"/>
       <c r="E9" s="82"/>
       <c r="F9" s="82"/>
     </row>
     <row r="10" spans="2:7" ht="18" customHeight="1">
       <c r="B10" s="18"/>
-      <c r="C10" s="199" t="s">
+      <c r="C10" s="178" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="200"/>
+      <c r="D10" s="179"/>
       <c r="E10" s="81"/>
       <c r="F10" s="81"/>
     </row>
@@ -4786,606 +5022,1192 @@
       <c r="F11" s="81"/>
     </row>
     <row r="12" spans="2:7" ht="18" customHeight="1">
-      <c r="B12" s="201" t="s">
+      <c r="B12" s="180" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="202" t="s">
+      <c r="C12" s="181" t="s">
         <v>251</v>
       </c>
-      <c r="D12" s="203" t="s">
+      <c r="D12" s="182" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="204" t="s">
+      <c r="E12" s="183" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="204" t="s">
+      <c r="F12" s="183" t="s">
         <v>71</v>
       </c>
+      <c r="G12" s="183" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="13" spans="2:7" ht="18" customHeight="1">
-      <c r="B13" s="222" t="s">
+      <c r="B13" s="194" t="s">
         <v>252</v>
       </c>
-      <c r="C13" s="219"/>
-      <c r="D13" s="220"/>
-      <c r="E13" s="221"/>
-      <c r="F13" s="221"/>
+      <c r="C13" s="192"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="193"/>
+      <c r="F13" s="193"/>
+      <c r="G13" s="193"/>
     </row>
     <row r="14" spans="2:7" ht="48" thickBot="1">
-      <c r="B14" s="223" t="s">
+      <c r="B14" s="195" t="s">
+        <v>258</v>
+      </c>
+      <c r="C14" s="184" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="81"/>
+      <c r="E14" s="185"/>
+      <c r="F14" s="185"/>
+      <c r="G14" s="185"/>
+    </row>
+    <row r="15" spans="2:7" ht="15.75" customHeight="1" thickTop="1">
+      <c r="B15" s="201"/>
+      <c r="C15" s="187"/>
+      <c r="D15" s="188" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="204" t="s">
+        <v>273</v>
+      </c>
+      <c r="F15" s="204" t="s">
+        <v>274</v>
+      </c>
+      <c r="G15" s="204" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B16" s="202" t="s">
+        <v>255</v>
+      </c>
+      <c r="C16" s="196" t="s">
+        <v>253</v>
+      </c>
+      <c r="D16" s="189" t="s">
+        <v>275</v>
+      </c>
+      <c r="E16" s="190"/>
+      <c r="F16" s="190"/>
+      <c r="G16" s="190"/>
+    </row>
+    <row r="17" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B17" s="202"/>
+      <c r="C17" s="196"/>
+      <c r="D17" s="189"/>
+      <c r="E17" s="190"/>
+      <c r="F17" s="190" t="s">
+        <v>276</v>
+      </c>
+      <c r="G17" s="190"/>
+    </row>
+    <row r="18" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B18" s="202"/>
+      <c r="C18" s="196"/>
+      <c r="D18" s="189"/>
+      <c r="E18" s="190"/>
+      <c r="F18" s="190"/>
+      <c r="G18" s="190"/>
+    </row>
+    <row r="19" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B19" s="202" t="s">
+        <v>264</v>
+      </c>
+      <c r="C19" s="196" t="s">
+        <v>296</v>
+      </c>
+      <c r="D19" s="189"/>
+      <c r="E19" s="190" t="s">
+        <v>292</v>
+      </c>
+      <c r="F19" s="190"/>
+      <c r="G19" s="190"/>
+    </row>
+    <row r="20" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B20" s="202"/>
+      <c r="C20" s="196"/>
+      <c r="D20" s="189"/>
+      <c r="E20" s="190" t="s">
+        <v>293</v>
+      </c>
+      <c r="F20" s="190"/>
+      <c r="G20" s="190"/>
+    </row>
+    <row r="21" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B21" s="201"/>
+      <c r="C21" s="186"/>
+      <c r="D21" s="189"/>
+      <c r="E21" s="190" t="s">
+        <v>277</v>
+      </c>
+      <c r="F21" s="190"/>
+      <c r="G21" s="190"/>
+    </row>
+    <row r="22" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B22" s="201"/>
+      <c r="C22" s="186"/>
+      <c r="D22" s="189"/>
+      <c r="E22" s="190" t="s">
+        <v>365</v>
+      </c>
+      <c r="F22" s="190"/>
+      <c r="G22" s="190"/>
+    </row>
+    <row r="23" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B23" s="201"/>
+      <c r="C23" s="186"/>
+      <c r="D23" s="189"/>
+      <c r="E23" s="190" t="s">
+        <v>282</v>
+      </c>
+      <c r="F23" s="190"/>
+      <c r="G23" s="190"/>
+    </row>
+    <row r="24" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B24" s="202" t="s">
+        <v>255</v>
+      </c>
+      <c r="C24" s="196" t="s">
+        <v>254</v>
+      </c>
+      <c r="D24" s="189" t="s">
+        <v>278</v>
+      </c>
+      <c r="E24" s="190"/>
+      <c r="F24" s="190"/>
+      <c r="G24" s="190"/>
+    </row>
+    <row r="25" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B25" s="202"/>
+      <c r="C25" s="196"/>
+      <c r="D25" s="189"/>
+      <c r="E25" s="190"/>
+      <c r="F25" s="190" t="s">
+        <v>279</v>
+      </c>
+      <c r="G25" s="190"/>
+    </row>
+    <row r="26" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B26" s="202"/>
+      <c r="C26" s="196"/>
+      <c r="D26" s="189"/>
+      <c r="E26" s="190"/>
+      <c r="F26" s="190"/>
+      <c r="G26" s="190"/>
+    </row>
+    <row r="27" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B27" s="202" t="s">
+        <v>264</v>
+      </c>
+      <c r="C27" s="196" t="s">
+        <v>297</v>
+      </c>
+      <c r="D27" s="189"/>
+      <c r="E27" s="190" t="s">
+        <v>294</v>
+      </c>
+      <c r="F27" s="190"/>
+      <c r="G27" s="190"/>
+    </row>
+    <row r="28" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B28" s="202"/>
+      <c r="C28" s="196"/>
+      <c r="D28" s="189"/>
+      <c r="E28" s="190" t="s">
+        <v>295</v>
+      </c>
+      <c r="F28" s="190"/>
+      <c r="G28" s="190"/>
+    </row>
+    <row r="29" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B29" s="202" t="s">
+        <v>264</v>
+      </c>
+      <c r="C29" s="196" t="s">
+        <v>271</v>
+      </c>
+      <c r="D29" s="189"/>
+      <c r="E29" s="190" t="s">
+        <v>280</v>
+      </c>
+      <c r="F29" s="190"/>
+      <c r="G29" s="190"/>
+    </row>
+    <row r="30" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B30" s="202"/>
+      <c r="C30" s="196"/>
+      <c r="D30" s="189"/>
+      <c r="E30" s="190" t="s">
+        <v>365</v>
+      </c>
+      <c r="F30" s="190"/>
+      <c r="G30" s="190"/>
+    </row>
+    <row r="31" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B31" s="202"/>
+      <c r="C31" s="196"/>
+      <c r="D31" s="189"/>
+      <c r="E31" s="190" t="s">
+        <v>281</v>
+      </c>
+      <c r="F31" s="190"/>
+      <c r="G31" s="190"/>
+    </row>
+    <row r="32" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B32" s="201"/>
+      <c r="C32" s="186"/>
+      <c r="D32" s="189"/>
+      <c r="E32" s="190" t="s">
+        <v>282</v>
+      </c>
+      <c r="F32" s="190"/>
+      <c r="G32" s="190"/>
+    </row>
+    <row r="33" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B33" s="202" t="s">
+        <v>255</v>
+      </c>
+      <c r="C33" s="196" t="s">
+        <v>256</v>
+      </c>
+      <c r="D33" s="189" t="s">
+        <v>290</v>
+      </c>
+      <c r="E33" s="190"/>
+      <c r="F33" s="190"/>
+      <c r="G33" s="190"/>
+    </row>
+    <row r="34" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B34" s="202"/>
+      <c r="C34" s="196"/>
+      <c r="D34" s="189" t="s">
+        <v>284</v>
+      </c>
+      <c r="E34" s="190"/>
+      <c r="F34" s="190"/>
+      <c r="G34" s="190"/>
+    </row>
+    <row r="35" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B35" s="202"/>
+      <c r="C35" s="196"/>
+      <c r="D35" s="189"/>
+      <c r="E35" s="190"/>
+      <c r="F35" s="190"/>
+      <c r="G35" s="190" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B36" s="202"/>
+      <c r="C36" s="196"/>
+      <c r="D36" s="189" t="s">
+        <v>283</v>
+      </c>
+      <c r="E36" s="190"/>
+      <c r="F36" s="190"/>
+      <c r="G36" s="190"/>
+    </row>
+    <row r="37" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B37" s="202"/>
+      <c r="C37" s="196"/>
+      <c r="D37" s="189"/>
+      <c r="E37" s="190"/>
+      <c r="F37" s="190" t="s">
+        <v>287</v>
+      </c>
+      <c r="G37" s="190"/>
+    </row>
+    <row r="38" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B38" s="202" t="s">
+        <v>262</v>
+      </c>
+      <c r="C38" s="196" t="s">
+        <v>335</v>
+      </c>
+      <c r="D38" s="189"/>
+      <c r="E38" s="190"/>
+      <c r="F38" s="190" t="s">
+        <v>289</v>
+      </c>
+      <c r="G38" s="190"/>
+    </row>
+    <row r="39" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B39" s="202"/>
+      <c r="C39" s="196"/>
+      <c r="D39" s="189"/>
+      <c r="E39" s="190"/>
+      <c r="F39" s="190" t="s">
+        <v>288</v>
+      </c>
+      <c r="G39" s="190"/>
+    </row>
+    <row r="40" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B40" s="202" t="s">
+        <v>264</v>
+      </c>
+      <c r="C40" s="196" t="s">
+        <v>298</v>
+      </c>
+      <c r="D40" s="189"/>
+      <c r="E40" s="190" t="s">
+        <v>291</v>
+      </c>
+      <c r="F40" s="190"/>
+      <c r="G40" s="190"/>
+    </row>
+    <row r="41" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B41" s="202"/>
+      <c r="C41" s="196"/>
+      <c r="D41" s="189"/>
+      <c r="E41" s="190" t="s">
+        <v>299</v>
+      </c>
+      <c r="F41" s="190"/>
+      <c r="G41" s="190"/>
+    </row>
+    <row r="42" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B42" s="202"/>
+      <c r="C42" s="196"/>
+      <c r="D42" s="189"/>
+      <c r="E42" s="190" t="s">
+        <v>300</v>
+      </c>
+      <c r="F42" s="190"/>
+      <c r="G42" s="190"/>
+    </row>
+    <row r="43" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B43" s="202"/>
+      <c r="C43" s="196"/>
+      <c r="D43" s="189"/>
+      <c r="E43" s="190" t="s">
+        <v>301</v>
+      </c>
+      <c r="F43" s="190"/>
+      <c r="G43" s="190"/>
+    </row>
+    <row r="44" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B44" s="202"/>
+      <c r="C44" s="196"/>
+      <c r="D44" s="189"/>
+      <c r="E44" s="190" t="s">
+        <v>302</v>
+      </c>
+      <c r="F44" s="190"/>
+      <c r="G44" s="190"/>
+    </row>
+    <row r="45" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B45" s="202" t="s">
+        <v>255</v>
+      </c>
+      <c r="C45" s="196" t="s">
+        <v>257</v>
+      </c>
+      <c r="D45" s="189" t="s">
+        <v>303</v>
+      </c>
+      <c r="E45" s="190"/>
+      <c r="F45" s="190"/>
+      <c r="G45" s="190"/>
+    </row>
+    <row r="46" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B46" s="202"/>
+      <c r="C46" s="196"/>
+      <c r="D46" s="189"/>
+      <c r="E46" s="190"/>
+      <c r="F46" s="190"/>
+      <c r="G46" s="190" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B47" s="201"/>
+      <c r="C47" s="186"/>
+      <c r="D47" s="189"/>
+      <c r="E47" s="190"/>
+      <c r="F47" s="190" t="s">
+        <v>304</v>
+      </c>
+      <c r="G47" s="190"/>
+    </row>
+    <row r="48" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B48" s="202" t="s">
+        <v>255</v>
+      </c>
+      <c r="C48" s="196" t="s">
+        <v>309</v>
+      </c>
+      <c r="D48" s="226" t="s">
+        <v>310</v>
+      </c>
+      <c r="E48" s="190"/>
+      <c r="F48" s="190"/>
+      <c r="G48" s="190"/>
+    </row>
+    <row r="49" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B49" s="202"/>
+      <c r="C49" s="196"/>
+      <c r="D49" s="226"/>
+      <c r="E49" s="190"/>
+      <c r="F49" s="227" t="s">
+        <v>311</v>
+      </c>
+      <c r="G49" s="190"/>
+    </row>
+    <row r="50" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B50" s="201" t="s">
+        <v>262</v>
+      </c>
+      <c r="C50" s="196" t="s">
+        <v>336</v>
+      </c>
+      <c r="D50" s="189"/>
+      <c r="E50" s="190"/>
+      <c r="F50" s="190" t="s">
+        <v>306</v>
+      </c>
+      <c r="G50" s="190"/>
+    </row>
+    <row r="51" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B51" s="201"/>
+      <c r="C51" s="186"/>
+      <c r="D51" s="189"/>
+      <c r="E51" s="190"/>
+      <c r="F51" s="190" t="s">
+        <v>307</v>
+      </c>
+      <c r="G51" s="190"/>
+    </row>
+    <row r="52" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B52" s="201" t="s">
+        <v>264</v>
+      </c>
+      <c r="C52" s="196" t="s">
+        <v>265</v>
+      </c>
+      <c r="D52" s="189"/>
+      <c r="E52" s="227" t="s">
+        <v>318</v>
+      </c>
+      <c r="F52" s="190"/>
+      <c r="G52" s="190"/>
+    </row>
+    <row r="53" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B53" s="201"/>
+      <c r="C53" s="186"/>
+      <c r="D53" s="189"/>
+      <c r="E53" s="227" t="s">
+        <v>312</v>
+      </c>
+      <c r="F53" s="190"/>
+      <c r="G53" s="190"/>
+    </row>
+    <row r="54" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B54" s="201"/>
+      <c r="C54" s="186"/>
+      <c r="D54" s="189"/>
+      <c r="E54" s="227" t="s">
+        <v>313</v>
+      </c>
+      <c r="F54" s="190"/>
+      <c r="G54" s="190"/>
+    </row>
+    <row r="55" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B55" s="201"/>
+      <c r="C55" s="186"/>
+      <c r="D55" s="189"/>
+      <c r="E55" s="227" t="s">
+        <v>314</v>
+      </c>
+      <c r="F55" s="190"/>
+      <c r="G55" s="190"/>
+    </row>
+    <row r="56" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B56" s="201"/>
+      <c r="C56" s="186"/>
+      <c r="D56" s="189"/>
+      <c r="E56" s="227" t="s">
+        <v>315</v>
+      </c>
+      <c r="F56" s="190"/>
+      <c r="G56" s="190"/>
+    </row>
+    <row r="57" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B57" s="201"/>
+      <c r="C57" s="186"/>
+      <c r="D57" s="189"/>
+      <c r="E57" s="227" t="s">
+        <v>362</v>
+      </c>
+      <c r="F57" s="190"/>
+      <c r="G57" s="190"/>
+    </row>
+    <row r="58" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B58" s="201"/>
+      <c r="C58" s="186"/>
+      <c r="D58" s="189"/>
+      <c r="E58" s="227" t="s">
+        <v>321</v>
+      </c>
+      <c r="F58" s="190"/>
+      <c r="G58" s="190"/>
+    </row>
+    <row r="59" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B59" s="201"/>
+      <c r="C59" s="186"/>
+      <c r="D59" s="189"/>
+      <c r="E59" s="227" t="s">
+        <v>282</v>
+      </c>
+      <c r="F59" s="190"/>
+      <c r="G59" s="190"/>
+    </row>
+    <row r="60" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B60" s="202" t="s">
+        <v>255</v>
+      </c>
+      <c r="C60" s="196" t="s">
+        <v>308</v>
+      </c>
+      <c r="D60" s="226" t="s">
+        <v>316</v>
+      </c>
+      <c r="E60" s="190"/>
+      <c r="F60" s="190"/>
+      <c r="G60" s="190"/>
+    </row>
+    <row r="61" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B61" s="202"/>
+      <c r="C61" s="196"/>
+      <c r="D61" s="189"/>
+      <c r="E61" s="190"/>
+      <c r="F61" s="227" t="s">
+        <v>317</v>
+      </c>
+      <c r="G61" s="190"/>
+    </row>
+    <row r="62" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B62" s="202" t="s">
+        <v>264</v>
+      </c>
+      <c r="C62" s="196" t="s">
+        <v>266</v>
+      </c>
+      <c r="D62" s="189"/>
+      <c r="E62" s="227" t="s">
+        <v>319</v>
+      </c>
+      <c r="F62" s="190"/>
+      <c r="G62" s="190"/>
+    </row>
+    <row r="63" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B63" s="202"/>
+      <c r="C63" s="196"/>
+      <c r="D63" s="189"/>
+      <c r="E63" s="227" t="s">
+        <v>320</v>
+      </c>
+      <c r="F63" s="190"/>
+      <c r="G63" s="190"/>
+    </row>
+    <row r="64" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B64" s="202" t="s">
+        <v>264</v>
+      </c>
+      <c r="C64" s="196" t="s">
+        <v>322</v>
+      </c>
+      <c r="D64" s="189"/>
+      <c r="E64" s="227" t="s">
+        <v>323</v>
+      </c>
+      <c r="F64" s="190"/>
+      <c r="G64" s="190"/>
+    </row>
+    <row r="65" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B65" s="202"/>
+      <c r="C65" s="196"/>
+      <c r="D65" s="189"/>
+      <c r="E65" s="227" t="s">
+        <v>325</v>
+      </c>
+      <c r="F65" s="190"/>
+      <c r="G65" s="190"/>
+    </row>
+    <row r="66" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B66" s="202"/>
+      <c r="C66" s="196"/>
+      <c r="D66" s="189"/>
+      <c r="E66" s="227" t="s">
+        <v>324</v>
+      </c>
+      <c r="F66" s="190"/>
+      <c r="G66" s="190"/>
+    </row>
+    <row r="67" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B67" s="202"/>
+      <c r="C67" s="196"/>
+      <c r="D67" s="189"/>
+      <c r="E67" s="227" t="s">
+        <v>327</v>
+      </c>
+      <c r="F67" s="190"/>
+      <c r="G67" s="190"/>
+    </row>
+    <row r="68" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B68" s="202"/>
+      <c r="C68" s="196"/>
+      <c r="D68" s="189"/>
+      <c r="E68" s="227" t="s">
+        <v>326</v>
+      </c>
+      <c r="F68" s="190"/>
+      <c r="G68" s="190"/>
+    </row>
+    <row r="69" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B69" s="202" t="s">
+        <v>255</v>
+      </c>
+      <c r="C69" s="196" t="s">
+        <v>333</v>
+      </c>
+      <c r="D69" s="189" t="s">
+        <v>328</v>
+      </c>
+      <c r="E69" s="227"/>
+      <c r="F69" s="190"/>
+      <c r="G69" s="190"/>
+    </row>
+    <row r="70" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B70" s="202"/>
+      <c r="C70" s="196"/>
+      <c r="D70" s="189" t="s">
+        <v>329</v>
+      </c>
+      <c r="E70" s="227"/>
+      <c r="F70" s="190"/>
+      <c r="G70" s="190"/>
+    </row>
+    <row r="71" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B71" s="202"/>
+      <c r="C71" s="196"/>
+      <c r="D71" s="189" t="s">
+        <v>334</v>
+      </c>
+      <c r="E71" s="227"/>
+      <c r="F71" s="190"/>
+      <c r="G71" s="190"/>
+    </row>
+    <row r="72" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B72" s="202"/>
+      <c r="C72" s="196"/>
+      <c r="D72" s="189"/>
+      <c r="E72" s="227"/>
+      <c r="F72" s="190"/>
+      <c r="G72" s="190" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B73" s="202"/>
+      <c r="C73" s="196"/>
+      <c r="D73" s="189" t="s">
+        <v>331</v>
+      </c>
+      <c r="E73" s="227"/>
+      <c r="F73" s="190"/>
+      <c r="G73" s="190"/>
+    </row>
+    <row r="74" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B74" s="202"/>
+      <c r="C74" s="196"/>
+      <c r="D74" s="189"/>
+      <c r="E74" s="227"/>
+      <c r="F74" s="190" t="s">
+        <v>332</v>
+      </c>
+      <c r="G74" s="190"/>
+    </row>
+    <row r="75" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B75" s="202" t="s">
+        <v>262</v>
+      </c>
+      <c r="C75" s="196" t="s">
+        <v>263</v>
+      </c>
+      <c r="D75" s="189"/>
+      <c r="E75" s="190"/>
+      <c r="F75" s="227" t="s">
+        <v>337</v>
+      </c>
+      <c r="G75" s="190"/>
+    </row>
+    <row r="76" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B76" s="201"/>
+      <c r="C76" s="186"/>
+      <c r="D76" s="189"/>
+      <c r="E76" s="190"/>
+      <c r="F76" s="227" t="s">
+        <v>338</v>
+      </c>
+      <c r="G76" s="190"/>
+    </row>
+    <row r="77" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B77" s="202" t="s">
+        <v>264</v>
+      </c>
+      <c r="C77" s="196" t="s">
+        <v>339</v>
+      </c>
+      <c r="D77" s="189"/>
+      <c r="E77" s="227" t="s">
+        <v>342</v>
+      </c>
+      <c r="F77" s="190"/>
+      <c r="G77" s="190"/>
+    </row>
+    <row r="78" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B78" s="201"/>
+      <c r="C78" s="186"/>
+      <c r="D78" s="189"/>
+      <c r="E78" s="227" t="s">
+        <v>340</v>
+      </c>
+      <c r="F78" s="190"/>
+      <c r="G78" s="190"/>
+    </row>
+    <row r="79" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B79" s="202"/>
+      <c r="C79" s="196"/>
+      <c r="D79" s="189"/>
+      <c r="E79" s="227" t="s">
+        <v>341</v>
+      </c>
+      <c r="F79" s="190"/>
+      <c r="G79" s="190"/>
+    </row>
+    <row r="80" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B80" s="202"/>
+      <c r="C80" s="196"/>
+      <c r="D80" s="189"/>
+      <c r="E80" s="227"/>
+      <c r="F80" s="190"/>
+      <c r="G80" s="190"/>
+    </row>
+    <row r="81" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B81" s="202" t="s">
+        <v>264</v>
+      </c>
+      <c r="C81" s="196" t="s">
+        <v>344</v>
+      </c>
+      <c r="D81" s="189"/>
+      <c r="E81" s="227" t="s">
+        <v>345</v>
+      </c>
+      <c r="F81" s="190"/>
+      <c r="G81" s="190"/>
+    </row>
+    <row r="82" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B82" s="202"/>
+      <c r="C82" s="196"/>
+      <c r="D82" s="189"/>
+      <c r="E82" s="227" t="s">
+        <v>346</v>
+      </c>
+      <c r="F82" s="190"/>
+      <c r="G82" s="190"/>
+    </row>
+    <row r="83" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B83" s="202"/>
+      <c r="C83" s="196"/>
+      <c r="D83" s="189"/>
+      <c r="E83" s="227"/>
+      <c r="F83" s="190"/>
+      <c r="G83" s="190"/>
+    </row>
+    <row r="84" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B84" s="202" t="s">
+        <v>264</v>
+      </c>
+      <c r="C84" s="196" t="s">
+        <v>343</v>
+      </c>
+      <c r="D84" s="189"/>
+      <c r="E84" s="227" t="s">
+        <v>347</v>
+      </c>
+      <c r="F84" s="190"/>
+      <c r="G84" s="190"/>
+    </row>
+    <row r="85" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B85" s="202"/>
+      <c r="C85" s="196"/>
+      <c r="D85" s="189"/>
+      <c r="E85" s="227" t="s">
+        <v>348</v>
+      </c>
+      <c r="F85" s="190"/>
+      <c r="G85" s="190"/>
+    </row>
+    <row r="86" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B86" s="202"/>
+      <c r="C86" s="196"/>
+      <c r="D86" s="189"/>
+      <c r="E86" s="227"/>
+      <c r="F86" s="190"/>
+      <c r="G86" s="190"/>
+    </row>
+    <row r="87" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B87" s="202" t="s">
+        <v>264</v>
+      </c>
+      <c r="C87" s="196" t="s">
+        <v>267</v>
+      </c>
+      <c r="D87" s="189"/>
+      <c r="E87" s="227" t="s">
+        <v>349</v>
+      </c>
+      <c r="F87" s="190"/>
+      <c r="G87" s="190"/>
+    </row>
+    <row r="88" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B88" s="201"/>
+      <c r="C88" s="186"/>
+      <c r="D88" s="189"/>
+      <c r="E88" s="227" t="s">
+        <v>350</v>
+      </c>
+      <c r="F88" s="190"/>
+      <c r="G88" s="190"/>
+    </row>
+    <row r="89" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B89" s="201"/>
+      <c r="C89" s="186"/>
+      <c r="D89" s="189"/>
+      <c r="E89" s="227" t="s">
+        <v>351</v>
+      </c>
+      <c r="F89" s="190"/>
+      <c r="G89" s="190"/>
+    </row>
+    <row r="90" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B90" s="201"/>
+      <c r="C90" s="186"/>
+      <c r="D90" s="189"/>
+      <c r="E90" s="227"/>
+      <c r="F90" s="190"/>
+      <c r="G90" s="190"/>
+    </row>
+    <row r="91" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B91" s="202" t="s">
+        <v>264</v>
+      </c>
+      <c r="C91" s="196" t="s">
+        <v>352</v>
+      </c>
+      <c r="D91" s="189"/>
+      <c r="E91" s="227" t="s">
+        <v>353</v>
+      </c>
+      <c r="F91" s="190"/>
+      <c r="G91" s="190"/>
+    </row>
+    <row r="92" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B92" s="201"/>
+      <c r="C92" s="186"/>
+      <c r="D92" s="189"/>
+      <c r="E92" s="227" t="s">
+        <v>354</v>
+      </c>
+      <c r="F92" s="190"/>
+      <c r="G92" s="190"/>
+    </row>
+    <row r="93" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B93" s="201"/>
+      <c r="C93" s="186"/>
+      <c r="D93" s="189"/>
+      <c r="E93" s="227"/>
+      <c r="F93" s="190"/>
+      <c r="G93" s="190"/>
+    </row>
+    <row r="94" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B94" s="202" t="s">
+        <v>264</v>
+      </c>
+      <c r="C94" s="196" t="s">
+        <v>269</v>
+      </c>
+      <c r="D94" s="189"/>
+      <c r="E94" s="227" t="s">
+        <v>356</v>
+      </c>
+      <c r="F94" s="190"/>
+      <c r="G94" s="190"/>
+    </row>
+    <row r="95" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B95" s="202"/>
+      <c r="C95" s="196"/>
+      <c r="D95" s="189"/>
+      <c r="E95" s="227" t="s">
+        <v>355</v>
+      </c>
+      <c r="F95" s="190"/>
+      <c r="G95" s="190"/>
+    </row>
+    <row r="96" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B96" s="202"/>
+      <c r="C96" s="196"/>
+      <c r="D96" s="189"/>
+      <c r="E96" s="227" t="s">
+        <v>357</v>
+      </c>
+      <c r="F96" s="190"/>
+      <c r="G96" s="190"/>
+    </row>
+    <row r="97" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B97" s="201"/>
+      <c r="C97" s="186"/>
+      <c r="D97" s="189"/>
+      <c r="E97" s="227" t="s">
+        <v>358</v>
+      </c>
+      <c r="F97" s="190"/>
+      <c r="G97" s="190"/>
+    </row>
+    <row r="98" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B98" s="201"/>
+      <c r="C98" s="186"/>
+      <c r="D98" s="189"/>
+      <c r="E98" s="227"/>
+      <c r="F98" s="190"/>
+      <c r="G98" s="190"/>
+    </row>
+    <row r="99" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B99" s="202" t="s">
+        <v>264</v>
+      </c>
+      <c r="C99" s="196" t="s">
+        <v>268</v>
+      </c>
+      <c r="D99" s="189"/>
+      <c r="E99" s="190" t="s">
+        <v>359</v>
+      </c>
+      <c r="F99" s="190"/>
+      <c r="G99" s="190"/>
+    </row>
+    <row r="100" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B100" s="201"/>
+      <c r="C100" s="186"/>
+      <c r="D100" s="189"/>
+      <c r="E100" s="190" t="s">
+        <v>360</v>
+      </c>
+      <c r="F100" s="190"/>
+      <c r="G100" s="190"/>
+    </row>
+    <row r="101" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B101" s="201"/>
+      <c r="C101" s="186"/>
+      <c r="D101" s="189"/>
+      <c r="E101" s="190"/>
+      <c r="F101" s="190"/>
+      <c r="G101" s="190"/>
+    </row>
+    <row r="102" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B102" s="202" t="s">
+        <v>264</v>
+      </c>
+      <c r="C102" s="196" t="s">
+        <v>272</v>
+      </c>
+      <c r="D102" s="189"/>
+      <c r="E102" s="190" t="s">
+        <v>363</v>
+      </c>
+      <c r="F102" s="190"/>
+      <c r="G102" s="190"/>
+    </row>
+    <row r="103" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B103" s="201"/>
+      <c r="C103" s="186"/>
+      <c r="D103" s="189"/>
+      <c r="E103" s="190" t="s">
+        <v>361</v>
+      </c>
+      <c r="F103" s="190"/>
+      <c r="G103" s="190"/>
+    </row>
+    <row r="104" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B104" s="201"/>
+      <c r="C104" s="186"/>
+      <c r="D104" s="189"/>
+      <c r="E104" s="190" t="s">
+        <v>364</v>
+      </c>
+      <c r="F104" s="190"/>
+      <c r="G104" s="190"/>
+    </row>
+    <row r="105" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B105" s="201"/>
+      <c r="C105" s="186"/>
+      <c r="D105" s="189"/>
+      <c r="E105" s="190"/>
+      <c r="F105" s="190"/>
+      <c r="G105" s="190"/>
+    </row>
+    <row r="106" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B106" s="202" t="s">
+        <v>264</v>
+      </c>
+      <c r="C106" s="196" t="s">
+        <v>270</v>
+      </c>
+      <c r="D106" s="189"/>
+      <c r="E106" s="190" t="s">
+        <v>366</v>
+      </c>
+      <c r="F106" s="190"/>
+      <c r="G106" s="190"/>
+    </row>
+    <row r="107" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B107" s="201"/>
+      <c r="C107" s="186"/>
+      <c r="D107" s="189"/>
+      <c r="E107" s="190" t="s">
+        <v>270</v>
+      </c>
+      <c r="F107" s="190"/>
+      <c r="G107" s="190"/>
+    </row>
+    <row r="108" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B108" s="201"/>
+      <c r="C108" s="186"/>
+      <c r="D108" s="189"/>
+      <c r="E108" s="190"/>
+      <c r="F108" s="190"/>
+      <c r="G108" s="190"/>
+    </row>
+    <row r="109" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B109" s="202" t="s">
+        <v>255</v>
+      </c>
+      <c r="C109" s="196" t="s">
+        <v>259</v>
+      </c>
+      <c r="D109" s="189" t="s">
+        <v>367</v>
+      </c>
+      <c r="E109" s="190"/>
+      <c r="F109" s="190"/>
+      <c r="G109" s="190"/>
+    </row>
+    <row r="110" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B110" s="201"/>
+      <c r="C110" s="186"/>
+      <c r="D110" s="189"/>
+      <c r="E110" s="190"/>
+      <c r="F110" s="190"/>
+      <c r="G110" s="190" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B111" s="202" t="s">
+        <v>255</v>
+      </c>
+      <c r="C111" s="196" t="s">
+        <v>260</v>
+      </c>
+      <c r="D111" s="189" t="s">
+        <v>368</v>
+      </c>
+      <c r="E111" s="190"/>
+      <c r="F111" s="190"/>
+      <c r="G111" s="190"/>
+    </row>
+    <row r="112" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B112" s="201"/>
+      <c r="C112" s="186"/>
+      <c r="D112" s="189"/>
+      <c r="E112" s="190"/>
+      <c r="F112" s="190"/>
+      <c r="G112" s="190" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B113" s="202" t="s">
+        <v>255</v>
+      </c>
+      <c r="C113" s="196" t="s">
         <v>261</v>
       </c>
-      <c r="C14" s="205" t="s">
-        <v>72</v>
-      </c>
-      <c r="D14" s="81"/>
-      <c r="E14" s="206"/>
-      <c r="F14" s="206"/>
-      <c r="G14" s="81"/>
-    </row>
-    <row r="15" spans="2:7" ht="15.75" customHeight="1" thickTop="1">
-      <c r="B15" s="229"/>
-      <c r="C15" s="208"/>
-      <c r="D15" s="209" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="233" t="s">
-        <v>280</v>
-      </c>
-      <c r="F15" s="233" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B16" s="230" t="s">
+      <c r="D113" s="189" t="s">
+        <v>370</v>
+      </c>
+      <c r="E113" s="190"/>
+      <c r="F113" s="190"/>
+      <c r="G113" s="190"/>
+    </row>
+    <row r="114" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B114" s="201"/>
+      <c r="C114" s="186"/>
+      <c r="D114" s="189"/>
+      <c r="E114" s="190"/>
+      <c r="F114" s="190"/>
+      <c r="G114" s="190" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B115" s="201" t="s">
         <v>255</v>
       </c>
-      <c r="C16" s="224" t="s">
-        <v>253</v>
-      </c>
-      <c r="D16" s="211"/>
-      <c r="E16" s="212"/>
-      <c r="F16" s="212"/>
-    </row>
-    <row r="17" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B17" s="229"/>
-      <c r="C17" s="207"/>
-      <c r="D17" s="211"/>
-      <c r="E17" s="212"/>
-      <c r="F17" s="212"/>
-    </row>
-    <row r="18" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B18" s="230" t="s">
-        <v>255</v>
-      </c>
-      <c r="C18" s="224" t="s">
-        <v>254</v>
-      </c>
-      <c r="D18" s="214"/>
-      <c r="E18" s="215"/>
-      <c r="F18" s="215"/>
-    </row>
-    <row r="19" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B19" s="229"/>
-      <c r="C19" s="207"/>
-      <c r="D19" s="214"/>
-      <c r="E19" s="215"/>
-      <c r="F19" s="215"/>
-    </row>
-    <row r="20" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B20" s="230" t="s">
-        <v>255</v>
-      </c>
-      <c r="C20" s="224" t="s">
-        <v>256</v>
-      </c>
-      <c r="D20" s="214"/>
-      <c r="E20" s="215"/>
-      <c r="F20" s="215"/>
-    </row>
-    <row r="21" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B21" s="229"/>
-      <c r="C21" s="207"/>
-      <c r="D21" s="214"/>
-      <c r="E21" s="215"/>
-      <c r="F21" s="215"/>
-    </row>
-    <row r="22" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B22" s="230" t="s">
-        <v>255</v>
-      </c>
-      <c r="C22" s="224" t="s">
-        <v>257</v>
-      </c>
-      <c r="D22" s="214"/>
-      <c r="E22" s="215"/>
-      <c r="F22" s="215"/>
-    </row>
-    <row r="23" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B23" s="229"/>
-      <c r="C23" s="207"/>
-      <c r="D23" s="214"/>
-      <c r="E23" s="215"/>
-      <c r="F23" s="215"/>
-    </row>
-    <row r="24" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B24" s="230" t="s">
-        <v>255</v>
-      </c>
-      <c r="C24" s="224" t="s">
-        <v>258</v>
-      </c>
-      <c r="D24" s="214"/>
-      <c r="E24" s="215"/>
-      <c r="F24" s="215"/>
-    </row>
-    <row r="25" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B25" s="229"/>
-      <c r="C25" s="207"/>
-      <c r="D25" s="214"/>
-      <c r="E25" s="215"/>
-      <c r="F25" s="215"/>
-    </row>
-    <row r="26" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B26" s="230" t="s">
-        <v>255</v>
-      </c>
-      <c r="C26" s="224" t="s">
-        <v>259</v>
-      </c>
-      <c r="D26" s="214"/>
-      <c r="E26" s="215"/>
-      <c r="F26" s="215"/>
-    </row>
-    <row r="27" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B27" s="229"/>
-      <c r="C27" s="207"/>
-      <c r="D27" s="214"/>
-      <c r="E27" s="215"/>
-      <c r="F27" s="215"/>
-    </row>
-    <row r="28" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B28" s="230" t="s">
-        <v>255</v>
-      </c>
-      <c r="C28" s="224" t="s">
-        <v>260</v>
-      </c>
-      <c r="D28" s="214"/>
-      <c r="E28" s="215"/>
-      <c r="F28" s="215"/>
-    </row>
-    <row r="29" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B29" s="229"/>
-      <c r="C29" s="207"/>
-      <c r="D29" s="214"/>
-      <c r="E29" s="215"/>
-      <c r="F29" s="215"/>
-    </row>
-    <row r="30" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B30" s="230" t="s">
-        <v>255</v>
-      </c>
-      <c r="C30" s="224" t="s">
-        <v>262</v>
-      </c>
-      <c r="D30" s="214"/>
-      <c r="E30" s="215"/>
-      <c r="F30" s="215"/>
-    </row>
-    <row r="31" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B31" s="229"/>
-      <c r="C31" s="207"/>
-      <c r="D31" s="214"/>
-      <c r="E31" s="215"/>
-      <c r="F31" s="215"/>
-    </row>
-    <row r="32" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B32" s="230" t="s">
-        <v>255</v>
-      </c>
-      <c r="C32" s="224" t="s">
-        <v>263</v>
-      </c>
-      <c r="D32" s="214"/>
-      <c r="E32" s="215"/>
-      <c r="F32" s="215"/>
-    </row>
-    <row r="33" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B33" s="229"/>
-      <c r="C33" s="207"/>
-      <c r="D33" s="214"/>
-      <c r="E33" s="215"/>
-      <c r="F33" s="215"/>
-    </row>
-    <row r="34" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B34" s="230" t="s">
-        <v>255</v>
-      </c>
-      <c r="C34" s="224" t="s">
-        <v>264</v>
-      </c>
-      <c r="D34" s="214"/>
-      <c r="E34" s="215"/>
-      <c r="F34" s="215"/>
-    </row>
-    <row r="35" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B35" s="229"/>
-      <c r="C35" s="207"/>
-      <c r="D35" s="214"/>
-      <c r="E35" s="215"/>
-      <c r="F35" s="215"/>
-    </row>
-    <row r="36" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B36" s="230" t="s">
-        <v>265</v>
-      </c>
-      <c r="C36" s="224" t="s">
-        <v>266</v>
-      </c>
-      <c r="D36" s="214"/>
-      <c r="E36" s="215"/>
-      <c r="F36" s="215"/>
-    </row>
-    <row r="37" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B37" s="229"/>
-      <c r="C37" s="207"/>
-      <c r="D37" s="214"/>
-      <c r="E37" s="215"/>
-      <c r="F37" s="215"/>
-    </row>
-    <row r="38" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B38" s="230" t="s">
-        <v>265</v>
-      </c>
-      <c r="C38" s="224" t="s">
-        <v>267</v>
-      </c>
-      <c r="D38" s="214"/>
-      <c r="E38" s="215"/>
-      <c r="F38" s="215"/>
-    </row>
-    <row r="39" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B39" s="229"/>
-      <c r="C39" s="207"/>
-      <c r="D39" s="214"/>
-      <c r="E39" s="215"/>
-      <c r="F39" s="215"/>
-    </row>
-    <row r="40" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B40" s="230" t="s">
-        <v>265</v>
-      </c>
-      <c r="C40" s="224" t="s">
-        <v>268</v>
-      </c>
-      <c r="D40" s="214"/>
-      <c r="E40" s="215"/>
-      <c r="F40" s="215"/>
-    </row>
-    <row r="41" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B41" s="229"/>
-      <c r="C41" s="207"/>
-      <c r="D41" s="214"/>
-      <c r="E41" s="215"/>
-      <c r="F41" s="215"/>
-    </row>
-    <row r="42" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B42" s="230" t="s">
-        <v>269</v>
-      </c>
-      <c r="C42" s="224" t="s">
-        <v>270</v>
-      </c>
-      <c r="D42" s="214"/>
-      <c r="E42" s="215"/>
-      <c r="F42" s="215"/>
-    </row>
-    <row r="43" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B43" s="229"/>
-      <c r="C43" s="207"/>
-      <c r="D43" s="214"/>
-      <c r="E43" s="215"/>
-      <c r="F43" s="215"/>
-    </row>
-    <row r="44" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B44" s="230" t="s">
-        <v>269</v>
-      </c>
-      <c r="C44" s="224" t="s">
-        <v>271</v>
-      </c>
-      <c r="D44" s="214"/>
-      <c r="E44" s="215"/>
-      <c r="F44" s="215"/>
-    </row>
-    <row r="45" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B45" s="229"/>
-      <c r="C45" s="207"/>
-      <c r="D45" s="214"/>
-      <c r="E45" s="215"/>
-      <c r="F45" s="215"/>
-    </row>
-    <row r="46" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B46" s="230" t="s">
-        <v>269</v>
-      </c>
-      <c r="C46" s="224" t="s">
-        <v>272</v>
-      </c>
-      <c r="D46" s="214"/>
-      <c r="E46" s="215"/>
-      <c r="F46" s="215"/>
-    </row>
-    <row r="47" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B47" s="229"/>
-      <c r="C47" s="207"/>
-      <c r="D47" s="214"/>
-      <c r="E47" s="215"/>
-      <c r="F47" s="215"/>
-    </row>
-    <row r="48" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B48" s="230" t="s">
-        <v>269</v>
-      </c>
-      <c r="C48" s="224" t="s">
-        <v>273</v>
-      </c>
-      <c r="D48" s="214"/>
-      <c r="E48" s="215"/>
-      <c r="F48" s="215"/>
-    </row>
-    <row r="49" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B49" s="229"/>
-      <c r="C49" s="207"/>
-      <c r="D49" s="214"/>
-      <c r="E49" s="215"/>
-      <c r="F49" s="215"/>
-    </row>
-    <row r="50" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B50" s="230" t="s">
-        <v>269</v>
-      </c>
-      <c r="C50" s="224" t="s">
-        <v>274</v>
-      </c>
-      <c r="D50" s="214"/>
-      <c r="E50" s="215"/>
-      <c r="F50" s="215"/>
-    </row>
-    <row r="51" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B51" s="229"/>
-      <c r="C51" s="207"/>
-      <c r="D51" s="214"/>
-      <c r="E51" s="215"/>
-      <c r="F51" s="215"/>
-    </row>
-    <row r="52" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B52" s="230" t="s">
-        <v>269</v>
-      </c>
-      <c r="C52" s="224" t="s">
-        <v>275</v>
-      </c>
-      <c r="D52" s="214"/>
-      <c r="E52" s="215"/>
-      <c r="F52" s="215"/>
-    </row>
-    <row r="53" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B53" s="229"/>
-      <c r="C53" s="207"/>
-      <c r="D53" s="214"/>
-      <c r="E53" s="215"/>
-      <c r="F53" s="215"/>
-    </row>
-    <row r="54" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B54" s="230" t="s">
-        <v>269</v>
-      </c>
-      <c r="C54" s="224" t="s">
-        <v>278</v>
-      </c>
-      <c r="D54" s="214"/>
-      <c r="E54" s="215"/>
-      <c r="F54" s="215"/>
-    </row>
-    <row r="55" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B55" s="229"/>
-      <c r="C55" s="207"/>
-      <c r="D55" s="214"/>
-      <c r="E55" s="215"/>
-      <c r="F55" s="215"/>
-    </row>
-    <row r="56" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B56" s="230" t="s">
-        <v>269</v>
-      </c>
-      <c r="C56" s="224" t="s">
-        <v>276</v>
-      </c>
-      <c r="D56" s="214"/>
-      <c r="E56" s="215"/>
-      <c r="F56" s="215"/>
-    </row>
-    <row r="57" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B57" s="229"/>
-      <c r="C57" s="207"/>
-      <c r="D57" s="214"/>
-      <c r="E57" s="215"/>
-      <c r="F57" s="215"/>
-    </row>
-    <row r="58" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B58" s="230" t="s">
-        <v>269</v>
-      </c>
-      <c r="C58" s="224" t="s">
-        <v>277</v>
-      </c>
-      <c r="D58" s="214"/>
-      <c r="E58" s="215"/>
-      <c r="F58" s="215"/>
-    </row>
-    <row r="59" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B59" s="229"/>
-      <c r="C59" s="207"/>
-      <c r="D59" s="214"/>
-      <c r="E59" s="215"/>
-      <c r="F59" s="215"/>
-    </row>
-    <row r="60" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B60" s="230" t="s">
-        <v>269</v>
-      </c>
-      <c r="C60" s="224" t="s">
-        <v>279</v>
-      </c>
-      <c r="D60" s="214"/>
-      <c r="E60" s="215"/>
-      <c r="F60" s="215"/>
-    </row>
-    <row r="61" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B61" s="229"/>
-      <c r="C61" s="207"/>
-      <c r="D61" s="214"/>
-      <c r="E61" s="215"/>
-      <c r="F61" s="215"/>
-    </row>
-    <row r="62" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B62" s="229"/>
-      <c r="C62" s="207"/>
-      <c r="D62" s="214"/>
-      <c r="E62" s="215"/>
-      <c r="F62" s="215"/>
-    </row>
-    <row r="63" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B63" s="229"/>
-      <c r="C63" s="207"/>
-      <c r="D63" s="214"/>
-      <c r="E63" s="215"/>
-      <c r="F63" s="215"/>
-    </row>
-    <row r="64" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B64" s="229"/>
-      <c r="C64" s="207"/>
-      <c r="D64" s="214"/>
-      <c r="E64" s="215"/>
-      <c r="F64" s="215"/>
-    </row>
-    <row r="65" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B65" s="229"/>
-      <c r="C65" s="207"/>
-      <c r="D65" s="214"/>
-      <c r="E65" s="215"/>
-      <c r="F65" s="215"/>
-    </row>
-    <row r="66" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B66" s="229"/>
-      <c r="C66" s="207"/>
-      <c r="D66" s="214"/>
-      <c r="E66" s="215"/>
-      <c r="F66" s="215"/>
-    </row>
-    <row r="67" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B67" s="229"/>
-      <c r="C67" s="207"/>
-      <c r="D67" s="214"/>
-      <c r="E67" s="215"/>
-      <c r="F67" s="215"/>
-    </row>
-    <row r="68" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B68" s="229"/>
-      <c r="C68" s="207"/>
-      <c r="D68" s="214"/>
-      <c r="E68" s="215"/>
-      <c r="F68" s="215"/>
-    </row>
-    <row r="69" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B69" s="229"/>
-      <c r="C69" s="207"/>
-      <c r="D69" s="214"/>
-      <c r="E69" s="215"/>
-      <c r="F69" s="215"/>
-    </row>
-    <row r="70" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B70" s="229"/>
-      <c r="C70" s="207"/>
-      <c r="D70" s="214"/>
-      <c r="E70" s="215"/>
-      <c r="F70" s="215"/>
-    </row>
-    <row r="71" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B71" s="229"/>
-      <c r="C71" s="207"/>
-      <c r="D71" s="214"/>
-      <c r="E71" s="215"/>
-      <c r="F71" s="215"/>
-    </row>
-    <row r="72" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B72" s="231"/>
-      <c r="C72" s="210"/>
-      <c r="D72" s="211"/>
-      <c r="E72" s="212"/>
-      <c r="F72" s="212"/>
-    </row>
-    <row r="73" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B73" s="231"/>
-      <c r="C73" s="213"/>
-      <c r="D73" s="211"/>
-      <c r="E73" s="212"/>
-      <c r="F73" s="212"/>
-    </row>
-    <row r="74" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B74" s="229"/>
-      <c r="C74" s="207"/>
-      <c r="D74" s="214"/>
-      <c r="E74" s="215"/>
-      <c r="F74" s="215"/>
-    </row>
-    <row r="75" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B75" s="229"/>
-      <c r="C75" s="207"/>
-      <c r="D75" s="214"/>
-      <c r="E75" s="215"/>
-      <c r="F75" s="215"/>
-    </row>
-    <row r="76" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B76" s="229"/>
-      <c r="C76" s="207"/>
-      <c r="D76" s="214"/>
-      <c r="E76" s="215"/>
-      <c r="F76" s="215"/>
-    </row>
-    <row r="77" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B77" s="229"/>
-      <c r="C77" s="207"/>
-      <c r="D77" s="214"/>
-      <c r="E77" s="215"/>
-      <c r="F77" s="215"/>
-    </row>
-    <row r="78" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B78" s="229"/>
-      <c r="C78" s="207"/>
-      <c r="D78" s="214"/>
-      <c r="E78" s="215"/>
-      <c r="F78" s="215"/>
-    </row>
-    <row r="79" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B79" s="229"/>
-      <c r="C79" s="207"/>
-      <c r="D79" s="214"/>
-      <c r="E79" s="215"/>
-      <c r="F79" s="215"/>
-    </row>
-    <row r="80" spans="2:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B80" s="232"/>
-      <c r="C80" s="216"/>
-      <c r="D80" s="217"/>
-      <c r="E80" s="218"/>
-      <c r="F80" s="218"/>
-    </row>
-    <row r="85" spans="4:4" ht="18" customHeight="1"/>
-    <row r="88" spans="4:4" ht="15.75" customHeight="1">
-      <c r="D88" s="82"/>
+      <c r="C115" s="196" t="s">
+        <v>373</v>
+      </c>
+      <c r="D115" s="226" t="s">
+        <v>374</v>
+      </c>
+      <c r="E115" s="190"/>
+      <c r="F115" s="190"/>
+      <c r="G115" s="190"/>
+    </row>
+    <row r="116" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B116" s="201"/>
+      <c r="C116" s="186"/>
+      <c r="D116" s="189"/>
+      <c r="E116" s="190"/>
+      <c r="F116" s="190"/>
+      <c r="G116" s="227" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="117" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B117" s="201"/>
+      <c r="C117" s="186"/>
+      <c r="D117" s="189"/>
+      <c r="E117" s="190"/>
+      <c r="F117" s="190"/>
+      <c r="G117" s="227" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B118" s="203"/>
+      <c r="C118" s="191"/>
+      <c r="D118" s="189"/>
+      <c r="E118" s="190"/>
+      <c r="F118" s="190"/>
+      <c r="G118" s="190"/>
+    </row>
+    <row r="123" spans="2:7" ht="18" customHeight="1"/>
+    <row r="126" spans="2:7" ht="15.75" customHeight="1">
+      <c r="D126" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5405,7 +6227,7 @@
   <dimension ref="G1:W28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="Y28" sqref="Y28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
@@ -5582,13 +6404,13 @@
       <c r="J11" s="82"/>
       <c r="K11" s="82"/>
       <c r="L11" s="82"/>
-      <c r="M11" s="174"/>
-      <c r="N11" s="166"/>
-      <c r="O11" s="166"/>
+      <c r="M11" s="218"/>
+      <c r="N11" s="206"/>
+      <c r="O11" s="206"/>
       <c r="P11" s="82"/>
       <c r="Q11" s="82"/>
-      <c r="R11" s="174"/>
-      <c r="S11" s="175"/>
+      <c r="R11" s="218"/>
+      <c r="S11" s="219"/>
     </row>
     <row r="12" spans="7:19" ht="15">
       <c r="G12" s="26"/>
@@ -5798,9 +6620,9 @@
       <c r="W23" s="82"/>
     </row>
     <row r="24" spans="7:23" ht="15">
-      <c r="G24" s="173"/>
-      <c r="H24" s="166"/>
-      <c r="I24" s="166"/>
+      <c r="G24" s="217"/>
+      <c r="H24" s="206"/>
+      <c r="I24" s="206"/>
       <c r="J24" s="82"/>
       <c r="K24" s="82"/>
       <c r="L24" s="82"/>
@@ -5836,9 +6658,9 @@
       <c r="W25" s="82"/>
     </row>
     <row r="26" spans="7:23" ht="15">
-      <c r="G26" s="173"/>
-      <c r="H26" s="166"/>
-      <c r="I26" s="166"/>
+      <c r="G26" s="217"/>
+      <c r="H26" s="206"/>
+      <c r="I26" s="206"/>
       <c r="J26" s="82"/>
       <c r="K26" s="82"/>
       <c r="L26" s="82"/>
@@ -5883,14 +6705,14 @@
       <c r="M28" s="82"/>
       <c r="N28" s="82"/>
       <c r="O28" s="82"/>
-      <c r="P28" s="173"/>
-      <c r="Q28" s="166"/>
-      <c r="R28" s="166"/>
+      <c r="P28" s="217"/>
+      <c r="Q28" s="206"/>
+      <c r="R28" s="206"/>
       <c r="S28" s="82"/>
-      <c r="T28" s="173"/>
-      <c r="U28" s="166"/>
-      <c r="V28" s="166"/>
-      <c r="W28" s="166"/>
+      <c r="T28" s="217"/>
+      <c r="U28" s="206"/>
+      <c r="V28" s="206"/>
+      <c r="W28" s="206"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -5940,16 +6762,16 @@
     </row>
     <row r="3" spans="2:10" ht="84" customHeight="1">
       <c r="B3" s="81"/>
-      <c r="C3" s="171" t="s">
+      <c r="C3" s="211" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="171"/>
-      <c r="E3" s="171"/>
-      <c r="F3" s="171"/>
-      <c r="G3" s="171"/>
-      <c r="H3" s="171"/>
-      <c r="I3" s="171"/>
-      <c r="J3" s="171"/>
+      <c r="D3" s="211"/>
+      <c r="E3" s="211"/>
+      <c r="F3" s="211"/>
+      <c r="G3" s="211"/>
+      <c r="H3" s="211"/>
+      <c r="I3" s="211"/>
+      <c r="J3" s="211"/>
     </row>
     <row r="4" spans="2:10" ht="12.75" customHeight="1">
       <c r="B4" s="102"/>
@@ -6116,7 +6938,7 @@
   <dimension ref="B2:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
@@ -6133,32 +6955,32 @@
       </c>
     </row>
     <row r="3" spans="2:11" ht="17.25" customHeight="1">
-      <c r="C3" s="179" t="s">
+      <c r="C3" s="223" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="179"/>
-      <c r="E3" s="179"/>
-      <c r="F3" s="179"/>
-      <c r="G3" s="179"/>
-      <c r="H3" s="179"/>
-      <c r="I3" s="179"/>
-      <c r="J3" s="179"/>
-      <c r="K3" s="179"/>
+      <c r="D3" s="223"/>
+      <c r="E3" s="223"/>
+      <c r="F3" s="223"/>
+      <c r="G3" s="223"/>
+      <c r="H3" s="223"/>
+      <c r="I3" s="223"/>
+      <c r="J3" s="223"/>
+      <c r="K3" s="223"/>
     </row>
     <row r="4" spans="2:11" ht="15" customHeight="1">
       <c r="C4" s="94"/>
     </row>
     <row r="5" spans="2:11" ht="12.75">
-      <c r="G5" s="177" t="s">
+      <c r="G5" s="221" t="s">
         <v>108</v>
       </c>
-      <c r="H5" s="178"/>
+      <c r="H5" s="222"/>
     </row>
     <row r="6" spans="2:11" ht="18.75" customHeight="1">
-      <c r="C6" s="176" t="s">
+      <c r="C6" s="220" t="s">
         <v>109</v>
       </c>
-      <c r="D6" s="176"/>
+      <c r="D6" s="220"/>
       <c r="G6" s="83" t="s">
         <v>110</v>
       </c>
@@ -6268,7 +7090,7 @@
   <dimension ref="B1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
@@ -6286,33 +7108,33 @@
     <row r="1" spans="2:8" ht="57" customHeight="1">
       <c r="B1" s="85"/>
       <c r="C1" s="86"/>
-      <c r="D1" s="180" t="s">
+      <c r="D1" s="224" t="s">
         <v>122</v>
       </c>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
+      <c r="E1" s="206"/>
+      <c r="F1" s="206"/>
+      <c r="G1" s="206"/>
+      <c r="H1" s="206"/>
     </row>
     <row r="2" spans="2:8" ht="12.75" customHeight="1">
       <c r="B2" s="85"/>
       <c r="C2" s="86"/>
-      <c r="D2" s="178" t="s">
+      <c r="D2" s="222" t="s">
         <v>123</v>
       </c>
-      <c r="E2" s="178"/>
-      <c r="F2" s="178"/>
-      <c r="G2" s="178"/>
-      <c r="H2" s="178"/>
+      <c r="E2" s="222"/>
+      <c r="F2" s="222"/>
+      <c r="G2" s="222"/>
+      <c r="H2" s="222"/>
     </row>
     <row r="3" spans="2:8" ht="12.75" customHeight="1">
       <c r="B3" s="85"/>
       <c r="C3" s="86"/>
-      <c r="D3" s="178"/>
-      <c r="E3" s="178"/>
-      <c r="F3" s="178"/>
-      <c r="G3" s="178"/>
-      <c r="H3" s="178"/>
+      <c r="D3" s="222"/>
+      <c r="E3" s="222"/>
+      <c r="F3" s="222"/>
+      <c r="G3" s="222"/>
+      <c r="H3" s="222"/>
     </row>
     <row r="4" spans="2:8" ht="12.75" customHeight="1">
       <c r="B4" s="39" t="s">
@@ -6435,12 +7257,12 @@
       <c r="E3" s="43"/>
       <c r="F3" s="43"/>
       <c r="G3" s="43"/>
-      <c r="H3" s="181"/>
-      <c r="I3" s="166"/>
-      <c r="J3" s="166"/>
-      <c r="K3" s="166"/>
-      <c r="L3" s="166"/>
-      <c r="M3" s="166"/>
+      <c r="H3" s="225"/>
+      <c r="I3" s="206"/>
+      <c r="J3" s="206"/>
+      <c r="K3" s="206"/>
+      <c r="L3" s="206"/>
+      <c r="M3" s="206"/>
     </row>
     <row r="4" spans="2:13" ht="21.75" customHeight="1">
       <c r="B4" s="74"/>

</xml_diff>